<commit_message>
Update pancreas millitome lookup
</commit_message>
<xml_diff>
--- a/staging/hubmap-pancreas_millitome-thompson-2024/resources/lookup3.0.xlsx
+++ b/staging/hubmap-pancreas_millitome-thompson-2024/resources/lookup3.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dequeue/Desktop/RUI.nosync/hra-registrations/staging/hubmap-pancreas_millitome-thompson-2024/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7B6385CA-D7D3-9E4E-8408-73BDF5AB0334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E11FE0AF-B24B-424C-AA0B-137D2E317019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="500" windowWidth="51200" windowHeight="26380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3002" uniqueCount="1782">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2554" uniqueCount="1724">
   <si>
     <t>Sample ID</t>
   </si>
@@ -4030,9 +4030,6 @@
     <t>874a4ff32cca87fc774d8b3125874976</t>
   </si>
   <si>
-    <t>https://purl.humanatlas.io/millitome/pancreas-female-uf/v1.0#3A1</t>
-  </si>
-  <si>
     <t>https://entity.api.hubmapconsortium.org/entities/109c9f0608cd6931e180c3199a3adfbb</t>
   </si>
   <si>
@@ -4048,9 +4045,6 @@
     <t>109c9f0608cd6931e180c3199a3adfbb</t>
   </si>
   <si>
-    <t>https://purl.humanatlas.io/millitome/pancreas-female-uf/v1.0#3A2</t>
-  </si>
-  <si>
     <t>https://entity.api.hubmapconsortium.org/entities/c0cc05d96e3de0a332d6f0c6a3ce4232</t>
   </si>
   <si>
@@ -4796,174 +4790,6 @@
   </si>
   <si>
     <t>https://purl.humanatlas.io/millitome/pancreas-female-uf/v1.0#25A</t>
-  </si>
-  <si>
-    <t>https://portal.hubmapconsortium.org/browse/donor/6f22d4528acc474a1abdc3596a341741</t>
-  </si>
-  <si>
-    <t>https://portal.hubmapconsortium.org/browse/donor/6f22d4528acc474a1abdc3596a341742</t>
-  </si>
-  <si>
-    <t>https://portal.hubmapconsortium.org/browse/donor/6f22d4528acc474a1abdc3596a341743</t>
-  </si>
-  <si>
-    <t>https://portal.hubmapconsortium.org/browse/donor/6f22d4528acc474a1abdc3596a341744</t>
-  </si>
-  <si>
-    <t>https://portal.hubmapconsortium.org/browse/donor/6f22d4528acc474a1abdc3596a341745</t>
-  </si>
-  <si>
-    <t>https://portal.hubmapconsortium.org/browse/donor/6f22d4528acc474a1abdc3596a341746</t>
-  </si>
-  <si>
-    <t>https://portal.hubmapconsortium.org/browse/donor/6f22d4528acc474a1abdc3596a341747</t>
-  </si>
-  <si>
-    <t>https://portal.hubmapconsortium.org/browse/donor/6f22d4528acc474a1abdc3596a341748</t>
-  </si>
-  <si>
-    <t>https://portal.hubmapconsortium.org/browse/donor/6f22d4528acc474a1abdc3596a341749</t>
-  </si>
-  <si>
-    <t>https://portal.hubmapconsortium.org/browse/donor/6f22d4528acc474a1abdc3596a341750</t>
-  </si>
-  <si>
-    <t>https://portal.hubmapconsortium.org/browse/donor/6f22d4528acc474a1abdc3596a341751</t>
-  </si>
-  <si>
-    <t>https://portal.hubmapconsortium.org/browse/donor/6f22d4528acc474a1abdc3596a341752</t>
-  </si>
-  <si>
-    <t>https://portal.hubmapconsortium.org/browse/donor/6f22d4528acc474a1abdc3596a341753</t>
-  </si>
-  <si>
-    <t>https://portal.hubmapconsortium.org/browse/donor/6f22d4528acc474a1abdc3596a341754</t>
-  </si>
-  <si>
-    <t>https://portal.hubmapconsortium.org/browse/donor/6f22d4528acc474a1abdc3596a341755</t>
-  </si>
-  <si>
-    <t>https://portal.hubmapconsortium.org/browse/donor/6f22d4528acc474a1abdc3596a341756</t>
-  </si>
-  <si>
-    <t>https://portal.hubmapconsortium.org/browse/donor/6f22d4528acc474a1abdc3596a341757</t>
-  </si>
-  <si>
-    <t>https://portal.hubmapconsortium.org/browse/donor/6f22d4528acc474a1abdc3596a341758</t>
-  </si>
-  <si>
-    <t>https://portal.hubmapconsortium.org/browse/donor/6f22d4528acc474a1abdc3596a341759</t>
-  </si>
-  <si>
-    <t>https://portal.hubmapconsortium.org/browse/donor/6f22d4528acc474a1abdc3596a341760</t>
-  </si>
-  <si>
-    <t>https://portal.hubmapconsortium.org/browse/donor/6f22d4528acc474a1abdc3596a341761</t>
-  </si>
-  <si>
-    <t>https://portal.hubmapconsortium.org/browse/donor/6f22d4528acc474a1abdc3596a341762</t>
-  </si>
-  <si>
-    <t>https://portal.hubmapconsortium.org/browse/donor/6f22d4528acc474a1abdc3596a341763</t>
-  </si>
-  <si>
-    <t>https://portal.hubmapconsortium.org/browse/donor/6f22d4528acc474a1abdc3596a341764</t>
-  </si>
-  <si>
-    <t>https://portal.hubmapconsortium.org/browse/donor/6f22d4528acc474a1abdc3596a341765</t>
-  </si>
-  <si>
-    <t>https://portal.hubmapconsortium.org/browse/donor/6f22d4528acc474a1abdc3596a341766</t>
-  </si>
-  <si>
-    <t>https://portal.hubmapconsortium.org/browse/donor/6f22d4528acc474a1abdc3596a341767</t>
-  </si>
-  <si>
-    <t>https://portal.hubmapconsortium.org/browse/donor/6f22d4528acc474a1abdc3596a341768</t>
-  </si>
-  <si>
-    <t>https://portal.hubmapconsortium.org/browse/donor/6f22d4528acc474a1abdc3596a341769</t>
-  </si>
-  <si>
-    <t>https://portal.hubmapconsortium.org/browse/donor/6f22d4528acc474a1abdc3596a341770</t>
-  </si>
-  <si>
-    <t>https://portal.hubmapconsortium.org/browse/donor/6f22d4528acc474a1abdc3596a341771</t>
-  </si>
-  <si>
-    <t>https://portal.hubmapconsortium.org/browse/donor/6f22d4528acc474a1abdc3596a341772</t>
-  </si>
-  <si>
-    <t>https://portal.hubmapconsortium.org/browse/donor/6f22d4528acc474a1abdc3596a341773</t>
-  </si>
-  <si>
-    <t>https://portal.hubmapconsortium.org/browse/donor/6f22d4528acc474a1abdc3596a341774</t>
-  </si>
-  <si>
-    <t>https://portal.hubmapconsortium.org/browse/donor/6f22d4528acc474a1abdc3596a341775</t>
-  </si>
-  <si>
-    <t>https://portal.hubmapconsortium.org/browse/donor/6f22d4528acc474a1abdc3596a341776</t>
-  </si>
-  <si>
-    <t>https://portal.hubmapconsortium.org/browse/donor/6f22d4528acc474a1abdc3596a341777</t>
-  </si>
-  <si>
-    <t>https://portal.hubmapconsortium.org/browse/donor/6f22d4528acc474a1abdc3596a341778</t>
-  </si>
-  <si>
-    <t>https://portal.hubmapconsortium.org/browse/donor/6f22d4528acc474a1abdc3596a341779</t>
-  </si>
-  <si>
-    <t>https://portal.hubmapconsortium.org/browse/donor/6f22d4528acc474a1abdc3596a341780</t>
-  </si>
-  <si>
-    <t>https://portal.hubmapconsortium.org/browse/donor/6f22d4528acc474a1abdc3596a341781</t>
-  </si>
-  <si>
-    <t>https://portal.hubmapconsortium.org/browse/donor/6f22d4528acc474a1abdc3596a341782</t>
-  </si>
-  <si>
-    <t>https://portal.hubmapconsortium.org/browse/donor/6f22d4528acc474a1abdc3596a341783</t>
-  </si>
-  <si>
-    <t>https://portal.hubmapconsortium.org/browse/donor/6f22d4528acc474a1abdc3596a341784</t>
-  </si>
-  <si>
-    <t>https://portal.hubmapconsortium.org/browse/donor/6f22d4528acc474a1abdc3596a341785</t>
-  </si>
-  <si>
-    <t>https://portal.hubmapconsortium.org/browse/donor/6f22d4528acc474a1abdc3596a341786</t>
-  </si>
-  <si>
-    <t>https://portal.hubmapconsortium.org/browse/donor/6f22d4528acc474a1abdc3596a341787</t>
-  </si>
-  <si>
-    <t>https://portal.hubmapconsortium.org/browse/donor/6f22d4528acc474a1abdc3596a341788</t>
-  </si>
-  <si>
-    <t>https://portal.hubmapconsortium.org/browse/donor/6f22d4528acc474a1abdc3596a341789</t>
-  </si>
-  <si>
-    <t>https://portal.hubmapconsortium.org/browse/donor/6f22d4528acc474a1abdc3596a341790</t>
-  </si>
-  <si>
-    <t>https://portal.hubmapconsortium.org/browse/donor/6f22d4528acc474a1abdc3596a341791</t>
-  </si>
-  <si>
-    <t>https://portal.hubmapconsortium.org/browse/donor/6f22d4528acc474a1abdc3596a341792</t>
-  </si>
-  <si>
-    <t>https://portal.hubmapconsortium.org/browse/donor/6f22d4528acc474a1abdc3596a341793</t>
-  </si>
-  <si>
-    <t>https://portal.hubmapconsortium.org/browse/donor/6f22d4528acc474a1abdc3596a341794</t>
-  </si>
-  <si>
-    <t>https://portal.hubmapconsortium.org/browse/donor/6f22d4528acc474a1abdc3596a341795</t>
-  </si>
-  <si>
-    <t>https://portal.hubmapconsortium.org/browse/donor/6f22d4528acc474a1abdc3596a341796</t>
   </si>
   <si>
     <t>https://entity.api.hubmapconsortium.org/entities/848f5662fc9791518ac4f77b3f7bc2c9</t>
@@ -5401,7 +5227,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5411,6 +5237,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5443,13 +5275,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -5753,10 +5586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O375"/>
+  <dimension ref="A1:O319"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A214" workbookViewId="0">
+      <selection activeCell="B223" sqref="B223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7142,34 +6975,34 @@
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+      <c r="A44" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E44" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F44">
+      <c r="F44" s="4">
         <v>17</v>
       </c>
-      <c r="G44">
+      <c r="G44" s="4">
         <v>18</v>
       </c>
-      <c r="H44" t="s">
+      <c r="H44" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="I44" t="s">
+      <c r="I44" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="J44" t="s">
+      <c r="J44" s="4" t="s">
         <v>268</v>
       </c>
     </row>
@@ -11070,7 +10903,7 @@
         <v>903</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>1781</v>
+        <v>1723</v>
       </c>
       <c r="C166" s="2" t="s">
         <v>904</v>
@@ -11094,7 +10927,7 @@
         <v>906</v>
       </c>
       <c r="J166" s="3" t="s">
-        <v>1653</v>
+        <v>1595</v>
       </c>
     </row>
     <row r="167" spans="1:10" x14ac:dyDescent="0.2">
@@ -11390,7 +11223,7 @@
         <v>955</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>1780</v>
+        <v>1722</v>
       </c>
       <c r="C176" s="2" t="s">
         <v>904</v>
@@ -11894,7 +11727,7 @@
         <v>1035</v>
       </c>
       <c r="J191" s="3" t="s">
-        <v>1413</v>
+        <v>1411</v>
       </c>
       <c r="K191" s="2"/>
       <c r="L191" s="2"/>
@@ -12677,7 +12510,7 @@
         <v>1163</v>
       </c>
       <c r="J215" s="3" t="s">
-        <v>1475</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="216" spans="1:10" x14ac:dyDescent="0.2">
@@ -12709,7 +12542,7 @@
         <v>1168</v>
       </c>
       <c r="J216" s="3" t="s">
-        <v>1475</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="217" spans="1:10" x14ac:dyDescent="0.2">
@@ -13609,81 +13442,81 @@
       </c>
     </row>
     <row r="245" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A245" t="s">
+      <c r="A245" s="2" t="s">
         <v>1331</v>
       </c>
-      <c r="B245" t="s">
+      <c r="B245" s="2" t="s">
         <v>1332</v>
       </c>
-      <c r="C245" t="s">
+      <c r="C245" s="2" t="s">
         <v>1301</v>
       </c>
-      <c r="D245" t="s">
+      <c r="D245" s="2" t="s">
         <v>1333</v>
       </c>
-      <c r="E245" t="s">
-        <v>597</v>
-      </c>
-      <c r="F245">
+      <c r="E245" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="F245" s="2">
         <v>48</v>
       </c>
-      <c r="G245">
+      <c r="G245" s="2">
         <v>24.8</v>
       </c>
-      <c r="H245" t="s">
+      <c r="H245" s="3" t="s">
         <v>1334</v>
       </c>
-      <c r="I245" t="s">
+      <c r="I245" s="2" t="s">
         <v>1335</v>
       </c>
-      <c r="J245" t="s">
+      <c r="J245" s="3" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="246" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A246" s="2" t="s">
         <v>1336</v>
       </c>
-    </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A246" t="s">
+      <c r="B246" s="2" t="s">
         <v>1337</v>
       </c>
-      <c r="B246" t="s">
+      <c r="C246" s="2" t="s">
+        <v>1301</v>
+      </c>
+      <c r="D246" s="2" t="s">
         <v>1338</v>
       </c>
-      <c r="C246" t="s">
-        <v>1301</v>
-      </c>
-      <c r="D246" t="s">
+      <c r="E246" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="F246" s="2">
+        <v>48</v>
+      </c>
+      <c r="G246" s="2">
+        <v>24.8</v>
+      </c>
+      <c r="H246" s="2" t="s">
         <v>1339</v>
       </c>
-      <c r="E246" t="s">
-        <v>597</v>
-      </c>
-      <c r="F246">
-        <v>48</v>
-      </c>
-      <c r="G246">
-        <v>24.8</v>
-      </c>
-      <c r="H246" t="s">
+      <c r="I246" s="2" t="s">
         <v>1340</v>
       </c>
-      <c r="I246" t="s">
-        <v>1341</v>
-      </c>
-      <c r="J246" t="s">
-        <v>1342</v>
+      <c r="J246" s="3" t="s">
+        <v>644</v>
       </c>
     </row>
     <row r="247" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
-        <v>1343</v>
+        <v>1341</v>
       </c>
       <c r="B247" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="C247" t="s">
         <v>1301</v>
       </c>
       <c r="D247" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="E247" t="s">
         <v>597</v>
@@ -13695,10 +13528,10 @@
         <v>24.8</v>
       </c>
       <c r="H247" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="I247" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="J247" t="s">
         <v>650</v>
@@ -13706,16 +13539,16 @@
     </row>
     <row r="248" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="B248" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="C248" t="s">
         <v>1301</v>
       </c>
       <c r="D248" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="E248" t="s">
         <v>597</v>
@@ -13727,10 +13560,10 @@
         <v>24.8</v>
       </c>
       <c r="H248" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="I248" t="s">
-        <v>1352</v>
+        <v>1350</v>
       </c>
       <c r="J248" t="s">
         <v>942</v>
@@ -13738,16 +13571,16 @@
     </row>
     <row r="249" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
-        <v>1353</v>
+        <v>1351</v>
       </c>
       <c r="B249" t="s">
-        <v>1354</v>
+        <v>1352</v>
       </c>
       <c r="C249" t="s">
         <v>1301</v>
       </c>
       <c r="D249" t="s">
-        <v>1355</v>
+        <v>1353</v>
       </c>
       <c r="E249" t="s">
         <v>597</v>
@@ -13759,10 +13592,10 @@
         <v>24.8</v>
       </c>
       <c r="H249" t="s">
-        <v>1356</v>
+        <v>1354</v>
       </c>
       <c r="I249" t="s">
-        <v>1357</v>
+        <v>1355</v>
       </c>
       <c r="J249" t="s">
         <v>656</v>
@@ -13770,16 +13603,16 @@
     </row>
     <row r="250" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
-        <v>1358</v>
+        <v>1356</v>
       </c>
       <c r="B250" t="s">
-        <v>1359</v>
+        <v>1357</v>
       </c>
       <c r="C250" t="s">
         <v>1301</v>
       </c>
       <c r="D250" t="s">
-        <v>1360</v>
+        <v>1358</v>
       </c>
       <c r="E250" t="s">
         <v>597</v>
@@ -13791,10 +13624,10 @@
         <v>24.8</v>
       </c>
       <c r="H250" t="s">
-        <v>1361</v>
+        <v>1359</v>
       </c>
       <c r="I250" t="s">
-        <v>1362</v>
+        <v>1360</v>
       </c>
       <c r="J250" t="s">
         <v>954</v>
@@ -13802,16 +13635,16 @@
     </row>
     <row r="251" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
-        <v>1363</v>
+        <v>1361</v>
       </c>
       <c r="B251" t="s">
-        <v>1364</v>
+        <v>1362</v>
       </c>
       <c r="C251" t="s">
         <v>1301</v>
       </c>
       <c r="D251" t="s">
-        <v>1365</v>
+        <v>1363</v>
       </c>
       <c r="E251" t="s">
         <v>597</v>
@@ -13823,10 +13656,10 @@
         <v>24.8</v>
       </c>
       <c r="H251" t="s">
-        <v>1366</v>
+        <v>1364</v>
       </c>
       <c r="I251" t="s">
-        <v>1367</v>
+        <v>1365</v>
       </c>
       <c r="J251" t="s">
         <v>680</v>
@@ -13834,16 +13667,16 @@
     </row>
     <row r="252" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
-        <v>1368</v>
+        <v>1366</v>
       </c>
       <c r="B252" t="s">
-        <v>1369</v>
+        <v>1367</v>
       </c>
       <c r="C252" t="s">
         <v>1301</v>
       </c>
       <c r="D252" t="s">
-        <v>1370</v>
+        <v>1368</v>
       </c>
       <c r="E252" t="s">
         <v>597</v>
@@ -13855,10 +13688,10 @@
         <v>24.8</v>
       </c>
       <c r="H252" t="s">
-        <v>1371</v>
+        <v>1369</v>
       </c>
       <c r="I252" t="s">
-        <v>1372</v>
+        <v>1370</v>
       </c>
       <c r="J252" t="s">
         <v>686</v>
@@ -13866,16 +13699,16 @@
     </row>
     <row r="253" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
-        <v>1373</v>
+        <v>1371</v>
       </c>
       <c r="B253" t="s">
-        <v>1374</v>
+        <v>1372</v>
       </c>
       <c r="C253" t="s">
         <v>1301</v>
       </c>
       <c r="D253" t="s">
-        <v>1375</v>
+        <v>1373</v>
       </c>
       <c r="E253" t="s">
         <v>597</v>
@@ -13887,10 +13720,10 @@
         <v>24.8</v>
       </c>
       <c r="H253" t="s">
-        <v>1376</v>
+        <v>1374</v>
       </c>
       <c r="I253" t="s">
-        <v>1377</v>
+        <v>1375</v>
       </c>
       <c r="J253" t="s">
         <v>692</v>
@@ -13898,16 +13731,16 @@
     </row>
     <row r="254" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
-        <v>1378</v>
+        <v>1376</v>
       </c>
       <c r="B254" t="s">
-        <v>1379</v>
+        <v>1377</v>
       </c>
       <c r="C254" t="s">
         <v>1301</v>
       </c>
       <c r="D254" t="s">
-        <v>1380</v>
+        <v>1378</v>
       </c>
       <c r="E254" t="s">
         <v>597</v>
@@ -13919,10 +13752,10 @@
         <v>24.8</v>
       </c>
       <c r="H254" t="s">
-        <v>1381</v>
+        <v>1379</v>
       </c>
       <c r="I254" t="s">
-        <v>1382</v>
+        <v>1380</v>
       </c>
       <c r="J254" t="s">
         <v>698</v>
@@ -13930,16 +13763,16 @@
     </row>
     <row r="255" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
-        <v>1383</v>
+        <v>1381</v>
       </c>
       <c r="B255" t="s">
-        <v>1384</v>
+        <v>1382</v>
       </c>
       <c r="C255" t="s">
         <v>1301</v>
       </c>
       <c r="D255" t="s">
-        <v>1385</v>
+        <v>1383</v>
       </c>
       <c r="E255" t="s">
         <v>597</v>
@@ -13951,10 +13784,10 @@
         <v>24.8</v>
       </c>
       <c r="H255" t="s">
-        <v>1386</v>
+        <v>1384</v>
       </c>
       <c r="I255" t="s">
-        <v>1387</v>
+        <v>1385</v>
       </c>
       <c r="J255" t="s">
         <v>704</v>
@@ -13962,16 +13795,16 @@
     </row>
     <row r="256" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
-        <v>1388</v>
+        <v>1386</v>
       </c>
       <c r="B256" t="s">
-        <v>1389</v>
+        <v>1387</v>
       </c>
       <c r="C256" t="s">
         <v>1301</v>
       </c>
       <c r="D256" t="s">
-        <v>1390</v>
+        <v>1388</v>
       </c>
       <c r="E256" t="s">
         <v>597</v>
@@ -13983,10 +13816,10 @@
         <v>24.8</v>
       </c>
       <c r="H256" t="s">
-        <v>1391</v>
+        <v>1389</v>
       </c>
       <c r="I256" t="s">
-        <v>1392</v>
+        <v>1390</v>
       </c>
       <c r="J256" t="s">
         <v>989</v>
@@ -13994,16 +13827,16 @@
     </row>
     <row r="257" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
-        <v>1393</v>
+        <v>1391</v>
       </c>
       <c r="B257" t="s">
-        <v>1394</v>
+        <v>1392</v>
       </c>
       <c r="C257" t="s">
         <v>1301</v>
       </c>
       <c r="D257" t="s">
-        <v>1395</v>
+        <v>1393</v>
       </c>
       <c r="E257" t="s">
         <v>597</v>
@@ -14015,10 +13848,10 @@
         <v>24.8</v>
       </c>
       <c r="H257" t="s">
-        <v>1396</v>
+        <v>1394</v>
       </c>
       <c r="I257" t="s">
-        <v>1397</v>
+        <v>1395</v>
       </c>
       <c r="J257" t="s">
         <v>1000</v>
@@ -14026,16 +13859,16 @@
     </row>
     <row r="258" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
-        <v>1398</v>
+        <v>1396</v>
       </c>
       <c r="B258" t="s">
-        <v>1399</v>
+        <v>1397</v>
       </c>
       <c r="C258" t="s">
         <v>1301</v>
       </c>
       <c r="D258" t="s">
-        <v>1400</v>
+        <v>1398</v>
       </c>
       <c r="E258" t="s">
         <v>597</v>
@@ -14047,10 +13880,10 @@
         <v>24.8</v>
       </c>
       <c r="H258" t="s">
-        <v>1401</v>
+        <v>1399</v>
       </c>
       <c r="I258" t="s">
-        <v>1402</v>
+        <v>1400</v>
       </c>
       <c r="J258" t="s">
         <v>740</v>
@@ -14058,16 +13891,16 @@
     </row>
     <row r="259" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
-        <v>1403</v>
+        <v>1401</v>
       </c>
       <c r="B259" t="s">
-        <v>1404</v>
+        <v>1402</v>
       </c>
       <c r="C259" t="s">
         <v>1301</v>
       </c>
       <c r="D259" t="s">
-        <v>1405</v>
+        <v>1403</v>
       </c>
       <c r="E259" t="s">
         <v>597</v>
@@ -14079,10 +13912,10 @@
         <v>24.8</v>
       </c>
       <c r="H259" t="s">
-        <v>1406</v>
+        <v>1404</v>
       </c>
       <c r="I259" t="s">
-        <v>1407</v>
+        <v>1405</v>
       </c>
       <c r="J259" t="s">
         <v>746</v>
@@ -14090,16 +13923,16 @@
     </row>
     <row r="260" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
-        <v>1408</v>
+        <v>1406</v>
       </c>
       <c r="B260" t="s">
-        <v>1409</v>
+        <v>1407</v>
       </c>
       <c r="C260" t="s">
         <v>1301</v>
       </c>
       <c r="D260" t="s">
-        <v>1410</v>
+        <v>1408</v>
       </c>
       <c r="E260" t="s">
         <v>597</v>
@@ -14111,27 +13944,27 @@
         <v>24.8</v>
       </c>
       <c r="H260" t="s">
+        <v>1409</v>
+      </c>
+      <c r="I260" t="s">
+        <v>1410</v>
+      </c>
+      <c r="J260" t="s">
         <v>1411</v>
-      </c>
-      <c r="I260" t="s">
-        <v>1412</v>
-      </c>
-      <c r="J260" t="s">
-        <v>1413</v>
       </c>
     </row>
     <row r="261" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="B261" t="s">
-        <v>1415</v>
+        <v>1413</v>
       </c>
       <c r="C261" t="s">
         <v>1301</v>
       </c>
       <c r="D261" t="s">
-        <v>1416</v>
+        <v>1414</v>
       </c>
       <c r="E261" t="s">
         <v>597</v>
@@ -14143,10 +13976,10 @@
         <v>24.8</v>
       </c>
       <c r="H261" t="s">
-        <v>1417</v>
+        <v>1415</v>
       </c>
       <c r="I261" t="s">
-        <v>1418</v>
+        <v>1416</v>
       </c>
       <c r="J261" t="s">
         <v>1051</v>
@@ -14154,16 +13987,16 @@
     </row>
     <row r="262" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
-        <v>1419</v>
+        <v>1417</v>
       </c>
       <c r="B262" t="s">
-        <v>1420</v>
+        <v>1418</v>
       </c>
       <c r="C262" t="s">
         <v>1301</v>
       </c>
       <c r="D262" t="s">
-        <v>1421</v>
+        <v>1419</v>
       </c>
       <c r="E262" t="s">
         <v>597</v>
@@ -14175,10 +14008,10 @@
         <v>24.8</v>
       </c>
       <c r="H262" t="s">
-        <v>1422</v>
+        <v>1420</v>
       </c>
       <c r="I262" t="s">
-        <v>1423</v>
+        <v>1421</v>
       </c>
       <c r="J262" t="s">
         <v>806</v>
@@ -14186,16 +14019,16 @@
     </row>
     <row r="263" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
-        <v>1424</v>
+        <v>1422</v>
       </c>
       <c r="B263" t="s">
-        <v>1425</v>
+        <v>1423</v>
       </c>
       <c r="C263" t="s">
         <v>1301</v>
       </c>
       <c r="D263" t="s">
-        <v>1426</v>
+        <v>1424</v>
       </c>
       <c r="E263" t="s">
         <v>597</v>
@@ -14207,10 +14040,10 @@
         <v>24.8</v>
       </c>
       <c r="H263" t="s">
-        <v>1427</v>
+        <v>1425</v>
       </c>
       <c r="I263" t="s">
-        <v>1428</v>
+        <v>1426</v>
       </c>
       <c r="J263" t="s">
         <v>812</v>
@@ -14218,16 +14051,16 @@
     </row>
     <row r="264" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
-        <v>1429</v>
+        <v>1427</v>
       </c>
       <c r="B264" t="s">
-        <v>1430</v>
+        <v>1428</v>
       </c>
       <c r="C264" t="s">
         <v>1301</v>
       </c>
       <c r="D264" t="s">
-        <v>1431</v>
+        <v>1429</v>
       </c>
       <c r="E264" t="s">
         <v>597</v>
@@ -14239,10 +14072,10 @@
         <v>24.8</v>
       </c>
       <c r="H264" t="s">
-        <v>1432</v>
+        <v>1430</v>
       </c>
       <c r="I264" t="s">
-        <v>1433</v>
+        <v>1431</v>
       </c>
       <c r="J264" t="s">
         <v>818</v>
@@ -14250,16 +14083,16 @@
     </row>
     <row r="265" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
-        <v>1434</v>
+        <v>1432</v>
       </c>
       <c r="B265" t="s">
-        <v>1435</v>
+        <v>1433</v>
       </c>
       <c r="C265" t="s">
         <v>1301</v>
       </c>
       <c r="D265" t="s">
-        <v>1436</v>
+        <v>1434</v>
       </c>
       <c r="E265" t="s">
         <v>597</v>
@@ -14271,10 +14104,10 @@
         <v>24.8</v>
       </c>
       <c r="H265" t="s">
-        <v>1437</v>
+        <v>1435</v>
       </c>
       <c r="I265" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="J265" t="s">
         <v>1094</v>
@@ -14282,16 +14115,16 @@
     </row>
     <row r="266" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
-        <v>1439</v>
+        <v>1437</v>
       </c>
       <c r="B266" t="s">
-        <v>1440</v>
+        <v>1438</v>
       </c>
       <c r="C266" t="s">
         <v>1301</v>
       </c>
       <c r="D266" t="s">
-        <v>1441</v>
+        <v>1439</v>
       </c>
       <c r="E266" t="s">
         <v>597</v>
@@ -14303,10 +14136,10 @@
         <v>24.8</v>
       </c>
       <c r="H266" t="s">
-        <v>1442</v>
+        <v>1440</v>
       </c>
       <c r="I266" t="s">
-        <v>1443</v>
+        <v>1441</v>
       </c>
       <c r="J266" t="s">
         <v>824</v>
@@ -14314,16 +14147,16 @@
     </row>
     <row r="267" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
-        <v>1444</v>
+        <v>1442</v>
       </c>
       <c r="B267" t="s">
-        <v>1445</v>
+        <v>1443</v>
       </c>
       <c r="C267" t="s">
         <v>1301</v>
       </c>
       <c r="D267" t="s">
-        <v>1446</v>
+        <v>1444</v>
       </c>
       <c r="E267" t="s">
         <v>597</v>
@@ -14335,10 +14168,10 @@
         <v>24.8</v>
       </c>
       <c r="H267" t="s">
-        <v>1447</v>
+        <v>1445</v>
       </c>
       <c r="I267" t="s">
-        <v>1448</v>
+        <v>1446</v>
       </c>
       <c r="J267" t="s">
         <v>830</v>
@@ -14346,16 +14179,16 @@
     </row>
     <row r="268" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
-        <v>1449</v>
+        <v>1447</v>
       </c>
       <c r="B268" t="s">
-        <v>1450</v>
+        <v>1448</v>
       </c>
       <c r="C268" t="s">
         <v>1301</v>
       </c>
       <c r="D268" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="E268" t="s">
         <v>597</v>
@@ -14367,27 +14200,27 @@
         <v>24.8</v>
       </c>
       <c r="H268" t="s">
+        <v>1450</v>
+      </c>
+      <c r="I268" t="s">
+        <v>1451</v>
+      </c>
+      <c r="J268" t="s">
         <v>1452</v>
-      </c>
-      <c r="I268" t="s">
-        <v>1453</v>
-      </c>
-      <c r="J268" t="s">
-        <v>1454</v>
       </c>
     </row>
     <row r="269" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
-        <v>1455</v>
+        <v>1453</v>
       </c>
       <c r="B269" t="s">
-        <v>1456</v>
+        <v>1454</v>
       </c>
       <c r="C269" t="s">
         <v>1301</v>
       </c>
       <c r="D269" t="s">
-        <v>1457</v>
+        <v>1455</v>
       </c>
       <c r="E269" t="s">
         <v>597</v>
@@ -14399,10 +14232,10 @@
         <v>24.8</v>
       </c>
       <c r="H269" t="s">
-        <v>1458</v>
+        <v>1456</v>
       </c>
       <c r="I269" t="s">
-        <v>1459</v>
+        <v>1457</v>
       </c>
       <c r="J269" t="s">
         <v>848</v>
@@ -14410,16 +14243,16 @@
     </row>
     <row r="270" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
-        <v>1460</v>
+        <v>1458</v>
       </c>
       <c r="B270" t="s">
-        <v>1461</v>
+        <v>1459</v>
       </c>
       <c r="C270" t="s">
         <v>1301</v>
       </c>
       <c r="D270" t="s">
-        <v>1462</v>
+        <v>1460</v>
       </c>
       <c r="E270" t="s">
         <v>597</v>
@@ -14431,10 +14264,10 @@
         <v>24.8</v>
       </c>
       <c r="H270" t="s">
-        <v>1463</v>
+        <v>1461</v>
       </c>
       <c r="I270" t="s">
-        <v>1464</v>
+        <v>1462</v>
       </c>
       <c r="J270" t="s">
         <v>854</v>
@@ -14442,16 +14275,16 @@
     </row>
     <row r="271" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
-        <v>1465</v>
+        <v>1463</v>
       </c>
       <c r="B271" t="s">
-        <v>1466</v>
+        <v>1464</v>
       </c>
       <c r="C271" t="s">
         <v>1301</v>
       </c>
       <c r="D271" t="s">
-        <v>1467</v>
+        <v>1465</v>
       </c>
       <c r="E271" t="s">
         <v>597</v>
@@ -14463,10 +14296,10 @@
         <v>24.8</v>
       </c>
       <c r="H271" t="s">
-        <v>1468</v>
+        <v>1466</v>
       </c>
       <c r="I271" t="s">
-        <v>1469</v>
+        <v>1467</v>
       </c>
       <c r="J271" t="s">
         <v>872</v>
@@ -14474,16 +14307,16 @@
     </row>
     <row r="272" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
-        <v>1470</v>
+        <v>1468</v>
       </c>
       <c r="B272" t="s">
-        <v>1471</v>
+        <v>1469</v>
       </c>
       <c r="C272" t="s">
         <v>1301</v>
       </c>
       <c r="D272" t="s">
-        <v>1472</v>
+        <v>1470</v>
       </c>
       <c r="E272" t="s">
         <v>597</v>
@@ -14495,27 +14328,27 @@
         <v>24.8</v>
       </c>
       <c r="H272" t="s">
+        <v>1471</v>
+      </c>
+      <c r="I272" t="s">
+        <v>1472</v>
+      </c>
+      <c r="J272" t="s">
         <v>1473</v>
-      </c>
-      <c r="I272" t="s">
-        <v>1474</v>
-      </c>
-      <c r="J272" t="s">
-        <v>1475</v>
       </c>
     </row>
     <row r="273" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
-        <v>1476</v>
+        <v>1474</v>
       </c>
       <c r="B273" t="s">
-        <v>1477</v>
+        <v>1475</v>
       </c>
       <c r="C273" t="s">
         <v>1301</v>
       </c>
       <c r="D273" t="s">
-        <v>1478</v>
+        <v>1476</v>
       </c>
       <c r="E273" t="s">
         <v>597</v>
@@ -14527,10 +14360,10 @@
         <v>24.8</v>
       </c>
       <c r="H273" t="s">
-        <v>1479</v>
+        <v>1477</v>
       </c>
       <c r="I273" t="s">
-        <v>1480</v>
+        <v>1478</v>
       </c>
       <c r="J273" t="s">
         <v>1179</v>
@@ -14538,16 +14371,16 @@
     </row>
     <row r="274" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
-        <v>1481</v>
+        <v>1479</v>
       </c>
       <c r="B274" t="s">
-        <v>1482</v>
+        <v>1480</v>
       </c>
       <c r="C274" t="s">
         <v>1301</v>
       </c>
       <c r="D274" t="s">
-        <v>1483</v>
+        <v>1481</v>
       </c>
       <c r="E274" t="s">
         <v>597</v>
@@ -14559,10 +14392,10 @@
         <v>24.8</v>
       </c>
       <c r="H274" t="s">
-        <v>1484</v>
+        <v>1482</v>
       </c>
       <c r="I274" t="s">
-        <v>1485</v>
+        <v>1483</v>
       </c>
       <c r="J274" t="s">
         <v>1185</v>
@@ -14570,16 +14403,16 @@
     </row>
     <row r="275" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
-        <v>1486</v>
+        <v>1484</v>
       </c>
       <c r="B275" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
       <c r="C275" t="s">
         <v>1301</v>
       </c>
       <c r="D275" t="s">
-        <v>1488</v>
+        <v>1486</v>
       </c>
       <c r="E275" t="s">
         <v>597</v>
@@ -14591,10 +14424,10 @@
         <v>24.8</v>
       </c>
       <c r="H275" t="s">
-        <v>1489</v>
+        <v>1487</v>
       </c>
       <c r="I275" t="s">
-        <v>1490</v>
+        <v>1488</v>
       </c>
       <c r="J275" t="s">
         <v>1191</v>
@@ -14602,16 +14435,16 @@
     </row>
     <row r="276" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
-        <v>1491</v>
+        <v>1489</v>
       </c>
       <c r="B276" t="s">
-        <v>1492</v>
+        <v>1490</v>
       </c>
       <c r="C276" t="s">
         <v>1301</v>
       </c>
       <c r="D276" t="s">
-        <v>1493</v>
+        <v>1491</v>
       </c>
       <c r="E276" t="s">
         <v>597</v>
@@ -14623,10 +14456,10 @@
         <v>24.8</v>
       </c>
       <c r="H276" t="s">
-        <v>1494</v>
+        <v>1492</v>
       </c>
       <c r="I276" t="s">
-        <v>1495</v>
+        <v>1493</v>
       </c>
       <c r="J276" t="s">
         <v>1197</v>
@@ -14634,16 +14467,16 @@
     </row>
     <row r="277" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
-        <v>1496</v>
+        <v>1494</v>
       </c>
       <c r="B277" t="s">
-        <v>1497</v>
+        <v>1495</v>
       </c>
       <c r="C277" t="s">
         <v>1301</v>
       </c>
       <c r="D277" t="s">
-        <v>1498</v>
+        <v>1496</v>
       </c>
       <c r="E277" t="s">
         <v>597</v>
@@ -14655,10 +14488,10 @@
         <v>24.8</v>
       </c>
       <c r="H277" t="s">
-        <v>1499</v>
+        <v>1497</v>
       </c>
       <c r="I277" t="s">
-        <v>1500</v>
+        <v>1498</v>
       </c>
       <c r="J277" t="s">
         <v>1203</v>
@@ -14666,16 +14499,16 @@
     </row>
     <row r="278" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
-        <v>1501</v>
+        <v>1499</v>
       </c>
       <c r="B278" t="s">
-        <v>1502</v>
+        <v>1500</v>
       </c>
       <c r="C278" t="s">
         <v>1301</v>
       </c>
       <c r="D278" t="s">
-        <v>1503</v>
+        <v>1501</v>
       </c>
       <c r="E278" t="s">
         <v>597</v>
@@ -14687,27 +14520,27 @@
         <v>24.8</v>
       </c>
       <c r="H278" t="s">
+        <v>1502</v>
+      </c>
+      <c r="I278" t="s">
+        <v>1503</v>
+      </c>
+      <c r="J278" t="s">
         <v>1504</v>
-      </c>
-      <c r="I278" t="s">
-        <v>1505</v>
-      </c>
-      <c r="J278" t="s">
-        <v>1506</v>
       </c>
     </row>
     <row r="279" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
-        <v>1507</v>
+        <v>1505</v>
       </c>
       <c r="B279" t="s">
-        <v>1508</v>
+        <v>1506</v>
       </c>
       <c r="C279" t="s">
         <v>1301</v>
       </c>
       <c r="D279" t="s">
-        <v>1509</v>
+        <v>1507</v>
       </c>
       <c r="E279" t="s">
         <v>597</v>
@@ -14719,27 +14552,27 @@
         <v>24.8</v>
       </c>
       <c r="H279" t="s">
+        <v>1508</v>
+      </c>
+      <c r="I279" t="s">
+        <v>1509</v>
+      </c>
+      <c r="J279" t="s">
         <v>1510</v>
-      </c>
-      <c r="I279" t="s">
-        <v>1511</v>
-      </c>
-      <c r="J279" t="s">
-        <v>1512</v>
       </c>
     </row>
     <row r="280" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
-        <v>1513</v>
+        <v>1511</v>
       </c>
       <c r="B280" t="s">
-        <v>1514</v>
+        <v>1512</v>
       </c>
       <c r="C280" t="s">
         <v>1301</v>
       </c>
       <c r="D280" t="s">
-        <v>1515</v>
+        <v>1513</v>
       </c>
       <c r="E280" t="s">
         <v>597</v>
@@ -14751,27 +14584,27 @@
         <v>24.8</v>
       </c>
       <c r="H280" t="s">
+        <v>1514</v>
+      </c>
+      <c r="I280" t="s">
+        <v>1515</v>
+      </c>
+      <c r="J280" t="s">
         <v>1516</v>
-      </c>
-      <c r="I280" t="s">
-        <v>1517</v>
-      </c>
-      <c r="J280" t="s">
-        <v>1518</v>
       </c>
     </row>
     <row r="281" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
-        <v>1519</v>
+        <v>1517</v>
       </c>
       <c r="B281" t="s">
-        <v>1520</v>
+        <v>1518</v>
       </c>
       <c r="C281" t="s">
         <v>1301</v>
       </c>
       <c r="D281" t="s">
-        <v>1521</v>
+        <v>1519</v>
       </c>
       <c r="E281" t="s">
         <v>597</v>
@@ -14783,10 +14616,10 @@
         <v>24.8</v>
       </c>
       <c r="H281" t="s">
-        <v>1522</v>
+        <v>1520</v>
       </c>
       <c r="I281" t="s">
-        <v>1523</v>
+        <v>1521</v>
       </c>
       <c r="J281" t="s">
         <v>1226</v>
@@ -14794,16 +14627,16 @@
     </row>
     <row r="282" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
-        <v>1524</v>
+        <v>1522</v>
       </c>
       <c r="B282" t="s">
-        <v>1525</v>
+        <v>1523</v>
       </c>
       <c r="C282" t="s">
         <v>1301</v>
       </c>
       <c r="D282" t="s">
-        <v>1526</v>
+        <v>1524</v>
       </c>
       <c r="E282" t="s">
         <v>597</v>
@@ -14815,10 +14648,10 @@
         <v>24.8</v>
       </c>
       <c r="H282" t="s">
-        <v>1527</v>
+        <v>1525</v>
       </c>
       <c r="I282" t="s">
-        <v>1528</v>
+        <v>1526</v>
       </c>
       <c r="J282" t="s">
         <v>1232</v>
@@ -14826,16 +14659,16 @@
     </row>
     <row r="283" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
-        <v>1529</v>
+        <v>1527</v>
       </c>
       <c r="B283" t="s">
-        <v>1530</v>
+        <v>1528</v>
       </c>
       <c r="C283" t="s">
         <v>1301</v>
       </c>
       <c r="D283" t="s">
-        <v>1531</v>
+        <v>1529</v>
       </c>
       <c r="E283" t="s">
         <v>597</v>
@@ -14847,10 +14680,10 @@
         <v>24.8</v>
       </c>
       <c r="H283" t="s">
-        <v>1532</v>
+        <v>1530</v>
       </c>
       <c r="I283" t="s">
-        <v>1533</v>
+        <v>1531</v>
       </c>
       <c r="J283" t="s">
         <v>1238</v>
@@ -14858,16 +14691,16 @@
     </row>
     <row r="284" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
-        <v>1534</v>
+        <v>1532</v>
       </c>
       <c r="B284" t="s">
-        <v>1535</v>
+        <v>1533</v>
       </c>
       <c r="C284" t="s">
         <v>1301</v>
       </c>
       <c r="D284" t="s">
-        <v>1536</v>
+        <v>1534</v>
       </c>
       <c r="E284" t="s">
         <v>597</v>
@@ -14879,10 +14712,10 @@
         <v>24.8</v>
       </c>
       <c r="H284" t="s">
-        <v>1537</v>
+        <v>1535</v>
       </c>
       <c r="I284" t="s">
-        <v>1538</v>
+        <v>1536</v>
       </c>
       <c r="J284" t="s">
         <v>1244</v>
@@ -14890,16 +14723,16 @@
     </row>
     <row r="285" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
-        <v>1539</v>
+        <v>1537</v>
       </c>
       <c r="B285" t="s">
-        <v>1540</v>
+        <v>1538</v>
       </c>
       <c r="C285" t="s">
         <v>1301</v>
       </c>
       <c r="D285" t="s">
-        <v>1541</v>
+        <v>1539</v>
       </c>
       <c r="E285" t="s">
         <v>597</v>
@@ -14911,27 +14744,27 @@
         <v>24.8</v>
       </c>
       <c r="H285" t="s">
+        <v>1540</v>
+      </c>
+      <c r="I285" t="s">
+        <v>1541</v>
+      </c>
+      <c r="J285" t="s">
         <v>1542</v>
-      </c>
-      <c r="I285" t="s">
-        <v>1543</v>
-      </c>
-      <c r="J285" t="s">
-        <v>1544</v>
       </c>
     </row>
     <row r="286" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
-        <v>1545</v>
+        <v>1543</v>
       </c>
       <c r="B286" t="s">
-        <v>1546</v>
+        <v>1544</v>
       </c>
       <c r="C286" t="s">
         <v>1301</v>
       </c>
       <c r="D286" t="s">
-        <v>1547</v>
+        <v>1545</v>
       </c>
       <c r="E286" t="s">
         <v>597</v>
@@ -14943,10 +14776,10 @@
         <v>24.8</v>
       </c>
       <c r="H286" t="s">
-        <v>1548</v>
+        <v>1546</v>
       </c>
       <c r="I286" t="s">
-        <v>1549</v>
+        <v>1547</v>
       </c>
       <c r="J286" t="s">
         <v>1250</v>
@@ -14954,16 +14787,16 @@
     </row>
     <row r="287" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
-        <v>1550</v>
+        <v>1548</v>
       </c>
       <c r="B287" t="s">
-        <v>1551</v>
+        <v>1549</v>
       </c>
       <c r="C287" t="s">
         <v>1301</v>
       </c>
       <c r="D287" t="s">
-        <v>1552</v>
+        <v>1550</v>
       </c>
       <c r="E287" t="s">
         <v>597</v>
@@ -14975,10 +14808,10 @@
         <v>24.8</v>
       </c>
       <c r="H287" t="s">
-        <v>1553</v>
+        <v>1551</v>
       </c>
       <c r="I287" t="s">
-        <v>1554</v>
+        <v>1552</v>
       </c>
       <c r="J287" t="s">
         <v>1256</v>
@@ -14986,16 +14819,16 @@
     </row>
     <row r="288" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
-        <v>1555</v>
+        <v>1553</v>
       </c>
       <c r="B288" t="s">
-        <v>1556</v>
+        <v>1554</v>
       </c>
       <c r="C288" t="s">
         <v>1301</v>
       </c>
       <c r="D288" t="s">
-        <v>1557</v>
+        <v>1555</v>
       </c>
       <c r="E288" t="s">
         <v>597</v>
@@ -15007,10 +14840,10 @@
         <v>24.8</v>
       </c>
       <c r="H288" t="s">
-        <v>1558</v>
+        <v>1556</v>
       </c>
       <c r="I288" t="s">
-        <v>1559</v>
+        <v>1557</v>
       </c>
       <c r="J288" t="s">
         <v>1262</v>
@@ -15018,16 +14851,16 @@
     </row>
     <row r="289" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
-        <v>1560</v>
+        <v>1558</v>
       </c>
       <c r="B289" t="s">
-        <v>1561</v>
+        <v>1559</v>
       </c>
       <c r="C289" t="s">
         <v>1301</v>
       </c>
       <c r="D289" t="s">
-        <v>1562</v>
+        <v>1560</v>
       </c>
       <c r="E289" t="s">
         <v>597</v>
@@ -15039,10 +14872,10 @@
         <v>24.8</v>
       </c>
       <c r="H289" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
       <c r="I289" t="s">
-        <v>1564</v>
+        <v>1562</v>
       </c>
       <c r="J289" t="s">
         <v>1268</v>
@@ -15050,16 +14883,16 @@
     </row>
     <row r="290" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
-        <v>1565</v>
+        <v>1563</v>
       </c>
       <c r="B290" t="s">
-        <v>1566</v>
+        <v>1564</v>
       </c>
       <c r="C290" t="s">
         <v>1301</v>
       </c>
       <c r="D290" t="s">
-        <v>1567</v>
+        <v>1565</v>
       </c>
       <c r="E290" t="s">
         <v>597</v>
@@ -15071,10 +14904,10 @@
         <v>24.8</v>
       </c>
       <c r="H290" t="s">
-        <v>1568</v>
+        <v>1566</v>
       </c>
       <c r="I290" t="s">
-        <v>1569</v>
+        <v>1567</v>
       </c>
       <c r="J290" t="s">
         <v>1274</v>
@@ -15082,16 +14915,16 @@
     </row>
     <row r="291" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
-        <v>1570</v>
+        <v>1568</v>
       </c>
       <c r="B291" t="s">
-        <v>1571</v>
+        <v>1569</v>
       </c>
       <c r="C291" t="s">
         <v>1301</v>
       </c>
       <c r="D291" t="s">
-        <v>1572</v>
+        <v>1570</v>
       </c>
       <c r="E291" t="s">
         <v>597</v>
@@ -15103,10 +14936,10 @@
         <v>24.8</v>
       </c>
       <c r="H291" t="s">
-        <v>1573</v>
+        <v>1571</v>
       </c>
       <c r="I291" t="s">
-        <v>1574</v>
+        <v>1572</v>
       </c>
       <c r="J291" t="s">
         <v>1280</v>
@@ -15114,16 +14947,16 @@
     </row>
     <row r="292" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
-        <v>1575</v>
+        <v>1573</v>
       </c>
       <c r="B292" t="s">
-        <v>1576</v>
+        <v>1574</v>
       </c>
       <c r="C292" t="s">
         <v>1301</v>
       </c>
       <c r="D292" t="s">
-        <v>1577</v>
+        <v>1575</v>
       </c>
       <c r="E292" t="s">
         <v>597</v>
@@ -15135,10 +14968,10 @@
         <v>24.8</v>
       </c>
       <c r="H292" t="s">
-        <v>1578</v>
+        <v>1576</v>
       </c>
       <c r="I292" t="s">
-        <v>1579</v>
+        <v>1577</v>
       </c>
       <c r="J292" t="s">
         <v>1286</v>
@@ -15146,16 +14979,16 @@
     </row>
     <row r="293" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
-        <v>1580</v>
+        <v>1578</v>
       </c>
       <c r="B293" t="s">
-        <v>1581</v>
+        <v>1579</v>
       </c>
       <c r="C293" t="s">
         <v>1301</v>
       </c>
       <c r="D293" t="s">
-        <v>1582</v>
+        <v>1580</v>
       </c>
       <c r="E293" t="s">
         <v>597</v>
@@ -15167,56 +15000,56 @@
         <v>24.8</v>
       </c>
       <c r="H293" t="s">
+        <v>1581</v>
+      </c>
+      <c r="I293" t="s">
+        <v>1582</v>
+      </c>
+      <c r="J293" t="s">
         <v>1583</v>
       </c>
-      <c r="I293" t="s">
+    </row>
+    <row r="294" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A294" s="4" t="s">
         <v>1584</v>
       </c>
-      <c r="J293" t="s">
+      <c r="B294" s="4" t="s">
         <v>1585</v>
       </c>
-    </row>
-    <row r="294" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A294" t="s">
+      <c r="C294" s="4" t="s">
+        <v>1301</v>
+      </c>
+      <c r="D294" s="4" t="s">
         <v>1586</v>
       </c>
-      <c r="B294" t="s">
+      <c r="E294" s="4" t="s">
+        <v>597</v>
+      </c>
+      <c r="F294" s="4">
+        <v>48</v>
+      </c>
+      <c r="G294" s="4">
+        <v>24.8</v>
+      </c>
+      <c r="H294" s="4" t="s">
         <v>1587</v>
       </c>
-      <c r="C294" t="s">
-        <v>1301</v>
-      </c>
-      <c r="D294" t="s">
+      <c r="I294" s="4" t="s">
         <v>1588</v>
       </c>
-      <c r="E294" t="s">
-        <v>597</v>
-      </c>
-      <c r="F294">
-        <v>48</v>
-      </c>
-      <c r="G294">
-        <v>24.8</v>
-      </c>
-      <c r="H294" t="s">
+      <c r="J294" s="4" t="s">
         <v>1589</v>
-      </c>
-      <c r="I294" t="s">
-        <v>1590</v>
-      </c>
-      <c r="J294" t="s">
-        <v>1591</v>
       </c>
     </row>
     <row r="295" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
-        <v>1299</v>
+        <v>1590</v>
       </c>
       <c r="B295" t="s">
-        <v>1300</v>
+        <v>1591</v>
       </c>
       <c r="C295" t="s">
-        <v>1301</v>
+        <v>1592</v>
       </c>
       <c r="D295" t="s">
         <v>1592</v>
@@ -15225,2578 +15058,786 @@
         <v>597</v>
       </c>
       <c r="F295">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G295">
-        <v>24.8</v>
+        <v>25.34</v>
       </c>
       <c r="H295" t="s">
-        <v>1302</v>
+        <v>1593</v>
       </c>
       <c r="I295" t="s">
-        <v>1303</v>
+        <v>1594</v>
       </c>
       <c r="J295" t="s">
-        <v>1304</v>
+        <v>1595</v>
       </c>
     </row>
     <row r="296" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
-        <v>1305</v>
+        <v>1596</v>
       </c>
       <c r="B296" t="s">
-        <v>1306</v>
+        <v>1597</v>
       </c>
       <c r="C296" t="s">
-        <v>1301</v>
+        <v>1592</v>
       </c>
       <c r="D296" t="s">
-        <v>1593</v>
+        <v>1598</v>
       </c>
       <c r="E296" t="s">
         <v>597</v>
       </c>
       <c r="F296">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G296">
-        <v>24.8</v>
+        <v>25.34</v>
       </c>
       <c r="H296" t="s">
-        <v>1308</v>
+        <v>1599</v>
       </c>
       <c r="I296" t="s">
-        <v>1309</v>
+        <v>1600</v>
       </c>
       <c r="J296" t="s">
-        <v>1310</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="297" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
-        <v>1311</v>
+        <v>1602</v>
       </c>
       <c r="B297" t="s">
-        <v>1312</v>
+        <v>1603</v>
       </c>
       <c r="C297" t="s">
-        <v>1301</v>
+        <v>1592</v>
       </c>
       <c r="D297" t="s">
-        <v>1594</v>
+        <v>1604</v>
       </c>
       <c r="E297" t="s">
         <v>597</v>
       </c>
       <c r="F297">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G297">
-        <v>24.8</v>
+        <v>25.34</v>
       </c>
       <c r="H297" t="s">
-        <v>1314</v>
+        <v>1605</v>
       </c>
       <c r="I297" t="s">
-        <v>1315</v>
+        <v>1606</v>
       </c>
       <c r="J297" t="s">
-        <v>620</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="298" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
-        <v>1316</v>
+        <v>1608</v>
       </c>
       <c r="B298" t="s">
-        <v>1317</v>
+        <v>1609</v>
       </c>
       <c r="C298" t="s">
-        <v>1301</v>
+        <v>1592</v>
       </c>
       <c r="D298" t="s">
-        <v>1595</v>
+        <v>1610</v>
       </c>
       <c r="E298" t="s">
         <v>597</v>
       </c>
       <c r="F298">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G298">
-        <v>24.8</v>
+        <v>25.34</v>
       </c>
       <c r="H298" t="s">
-        <v>1319</v>
+        <v>1611</v>
       </c>
       <c r="I298" t="s">
-        <v>1320</v>
+        <v>1612</v>
       </c>
       <c r="J298" t="s">
-        <v>626</v>
+        <v>1613</v>
       </c>
     </row>
     <row r="299" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
-        <v>1321</v>
+        <v>1614</v>
       </c>
       <c r="B299" t="s">
-        <v>1322</v>
+        <v>1615</v>
       </c>
       <c r="C299" t="s">
-        <v>1301</v>
+        <v>1592</v>
       </c>
       <c r="D299" t="s">
-        <v>1596</v>
+        <v>1616</v>
       </c>
       <c r="E299" t="s">
         <v>597</v>
       </c>
       <c r="F299">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G299">
-        <v>24.8</v>
+        <v>25.34</v>
       </c>
       <c r="H299" t="s">
-        <v>1324</v>
+        <v>1617</v>
       </c>
       <c r="I299" t="s">
-        <v>1325</v>
+        <v>1618</v>
       </c>
       <c r="J299" t="s">
-        <v>632</v>
+        <v>1619</v>
       </c>
     </row>
     <row r="300" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
-        <v>1326</v>
+        <v>1620</v>
       </c>
       <c r="B300" t="s">
-        <v>1327</v>
+        <v>1621</v>
       </c>
       <c r="C300" t="s">
-        <v>1301</v>
+        <v>1592</v>
       </c>
       <c r="D300" t="s">
-        <v>1597</v>
+        <v>1622</v>
       </c>
       <c r="E300" t="s">
         <v>597</v>
       </c>
       <c r="F300">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G300">
-        <v>24.8</v>
+        <v>25.34</v>
       </c>
       <c r="H300" t="s">
-        <v>1329</v>
+        <v>1623</v>
       </c>
       <c r="I300" t="s">
-        <v>1330</v>
+        <v>1624</v>
       </c>
       <c r="J300" t="s">
-        <v>638</v>
+        <v>1625</v>
       </c>
     </row>
     <row r="301" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
-        <v>1331</v>
+        <v>1626</v>
       </c>
       <c r="B301" t="s">
-        <v>1332</v>
+        <v>1627</v>
       </c>
       <c r="C301" t="s">
-        <v>1301</v>
+        <v>1592</v>
       </c>
       <c r="D301" t="s">
-        <v>1598</v>
+        <v>1628</v>
       </c>
       <c r="E301" t="s">
         <v>597</v>
       </c>
       <c r="F301">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G301">
-        <v>24.8</v>
+        <v>25.34</v>
       </c>
       <c r="H301" t="s">
-        <v>1334</v>
+        <v>1629</v>
       </c>
       <c r="I301" t="s">
-        <v>1335</v>
+        <v>1630</v>
       </c>
       <c r="J301" t="s">
-        <v>1336</v>
+        <v>954</v>
       </c>
     </row>
     <row r="302" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
-        <v>1337</v>
+        <v>1631</v>
       </c>
       <c r="B302" t="s">
-        <v>1338</v>
+        <v>1632</v>
       </c>
       <c r="C302" t="s">
-        <v>1301</v>
+        <v>1592</v>
       </c>
       <c r="D302" t="s">
-        <v>1599</v>
+        <v>1633</v>
       </c>
       <c r="E302" t="s">
         <v>597</v>
       </c>
       <c r="F302">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G302">
-        <v>24.8</v>
+        <v>25.34</v>
       </c>
       <c r="H302" t="s">
-        <v>1340</v>
+        <v>1634</v>
       </c>
       <c r="I302" t="s">
-        <v>1341</v>
+        <v>1635</v>
       </c>
       <c r="J302" t="s">
-        <v>1342</v>
+        <v>680</v>
       </c>
     </row>
     <row r="303" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
-        <v>1343</v>
+        <v>1636</v>
       </c>
       <c r="B303" t="s">
-        <v>1344</v>
+        <v>1637</v>
       </c>
       <c r="C303" t="s">
-        <v>1301</v>
+        <v>1592</v>
       </c>
       <c r="D303" t="s">
-        <v>1600</v>
+        <v>1638</v>
       </c>
       <c r="E303" t="s">
         <v>597</v>
       </c>
       <c r="F303">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G303">
-        <v>24.8</v>
+        <v>25.34</v>
       </c>
       <c r="H303" t="s">
-        <v>1346</v>
+        <v>1639</v>
       </c>
       <c r="I303" t="s">
-        <v>1347</v>
+        <v>1640</v>
       </c>
       <c r="J303" t="s">
-        <v>650</v>
+        <v>686</v>
       </c>
     </row>
     <row r="304" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
-        <v>1348</v>
+        <v>1641</v>
       </c>
       <c r="B304" t="s">
-        <v>1349</v>
+        <v>1642</v>
       </c>
       <c r="C304" t="s">
-        <v>1301</v>
+        <v>1592</v>
       </c>
       <c r="D304" t="s">
-        <v>1601</v>
+        <v>1643</v>
       </c>
       <c r="E304" t="s">
         <v>597</v>
       </c>
       <c r="F304">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G304">
-        <v>24.8</v>
+        <v>25.34</v>
       </c>
       <c r="H304" t="s">
-        <v>1351</v>
+        <v>1644</v>
       </c>
       <c r="I304" t="s">
-        <v>1352</v>
+        <v>1645</v>
       </c>
       <c r="J304" t="s">
-        <v>942</v>
+        <v>692</v>
       </c>
     </row>
     <row r="305" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
-        <v>1353</v>
+        <v>1646</v>
       </c>
       <c r="B305" t="s">
-        <v>1354</v>
+        <v>1647</v>
       </c>
       <c r="C305" t="s">
-        <v>1301</v>
+        <v>1592</v>
       </c>
       <c r="D305" t="s">
-        <v>1602</v>
+        <v>1648</v>
       </c>
       <c r="E305" t="s">
         <v>597</v>
       </c>
       <c r="F305">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G305">
-        <v>24.8</v>
+        <v>25.34</v>
       </c>
       <c r="H305" t="s">
-        <v>1356</v>
+        <v>1649</v>
       </c>
       <c r="I305" t="s">
-        <v>1357</v>
+        <v>1650</v>
       </c>
       <c r="J305" t="s">
-        <v>656</v>
+        <v>698</v>
       </c>
     </row>
     <row r="306" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
-        <v>1358</v>
+        <v>1651</v>
       </c>
       <c r="B306" t="s">
-        <v>1359</v>
+        <v>1652</v>
       </c>
       <c r="C306" t="s">
-        <v>1301</v>
+        <v>1592</v>
       </c>
       <c r="D306" t="s">
-        <v>1603</v>
+        <v>1653</v>
       </c>
       <c r="E306" t="s">
         <v>597</v>
       </c>
       <c r="F306">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G306">
-        <v>24.8</v>
+        <v>25.34</v>
       </c>
       <c r="H306" t="s">
-        <v>1361</v>
+        <v>1654</v>
       </c>
       <c r="I306" t="s">
-        <v>1362</v>
+        <v>1655</v>
       </c>
       <c r="J306" t="s">
-        <v>954</v>
+        <v>740</v>
       </c>
     </row>
     <row r="307" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
-        <v>1363</v>
+        <v>1656</v>
       </c>
       <c r="B307" t="s">
-        <v>1364</v>
+        <v>1657</v>
       </c>
       <c r="C307" t="s">
-        <v>1301</v>
+        <v>1592</v>
       </c>
       <c r="D307" t="s">
-        <v>1604</v>
+        <v>1658</v>
       </c>
       <c r="E307" t="s">
         <v>597</v>
       </c>
       <c r="F307">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G307">
-        <v>24.8</v>
+        <v>25.34</v>
       </c>
       <c r="H307" t="s">
-        <v>1366</v>
+        <v>1659</v>
       </c>
       <c r="I307" t="s">
-        <v>1367</v>
+        <v>1660</v>
       </c>
       <c r="J307" t="s">
-        <v>680</v>
+        <v>746</v>
       </c>
     </row>
     <row r="308" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
-        <v>1368</v>
+        <v>1661</v>
       </c>
       <c r="B308" t="s">
-        <v>1369</v>
+        <v>1662</v>
       </c>
       <c r="C308" t="s">
-        <v>1301</v>
+        <v>1592</v>
       </c>
       <c r="D308" t="s">
-        <v>1605</v>
+        <v>1663</v>
       </c>
       <c r="E308" t="s">
         <v>597</v>
       </c>
       <c r="F308">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G308">
-        <v>24.8</v>
+        <v>25.34</v>
       </c>
       <c r="H308" t="s">
-        <v>1371</v>
+        <v>1664</v>
       </c>
       <c r="I308" t="s">
-        <v>1372</v>
+        <v>1665</v>
       </c>
       <c r="J308" t="s">
-        <v>686</v>
+        <v>806</v>
       </c>
     </row>
     <row r="309" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
-        <v>1373</v>
+        <v>1666</v>
       </c>
       <c r="B309" t="s">
-        <v>1374</v>
+        <v>1667</v>
       </c>
       <c r="C309" t="s">
-        <v>1301</v>
+        <v>1592</v>
       </c>
       <c r="D309" t="s">
-        <v>1606</v>
+        <v>1668</v>
       </c>
       <c r="E309" t="s">
         <v>597</v>
       </c>
       <c r="F309">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G309">
-        <v>24.8</v>
+        <v>25.34</v>
       </c>
       <c r="H309" t="s">
-        <v>1376</v>
+        <v>1669</v>
       </c>
       <c r="I309" t="s">
-        <v>1377</v>
+        <v>1670</v>
       </c>
       <c r="J309" t="s">
-        <v>692</v>
+        <v>812</v>
       </c>
     </row>
     <row r="310" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
-        <v>1378</v>
+        <v>1671</v>
       </c>
       <c r="B310" t="s">
-        <v>1379</v>
+        <v>1672</v>
       </c>
       <c r="C310" t="s">
-        <v>1301</v>
+        <v>1592</v>
       </c>
       <c r="D310" t="s">
-        <v>1607</v>
+        <v>1673</v>
       </c>
       <c r="E310" t="s">
         <v>597</v>
       </c>
       <c r="F310">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G310">
-        <v>24.8</v>
+        <v>25.34</v>
       </c>
       <c r="H310" t="s">
-        <v>1381</v>
+        <v>1674</v>
       </c>
       <c r="I310" t="s">
-        <v>1382</v>
+        <v>1675</v>
       </c>
       <c r="J310" t="s">
-        <v>698</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="311" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
-        <v>1383</v>
+        <v>1676</v>
       </c>
       <c r="B311" t="s">
-        <v>1384</v>
+        <v>1677</v>
       </c>
       <c r="C311" t="s">
-        <v>1301</v>
+        <v>1592</v>
       </c>
       <c r="D311" t="s">
-        <v>1608</v>
+        <v>1678</v>
       </c>
       <c r="E311" t="s">
         <v>597</v>
       </c>
       <c r="F311">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G311">
-        <v>24.8</v>
+        <v>25.34</v>
       </c>
       <c r="H311" t="s">
-        <v>1386</v>
+        <v>1679</v>
       </c>
       <c r="I311" t="s">
-        <v>1387</v>
+        <v>1680</v>
       </c>
       <c r="J311" t="s">
-        <v>704</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="312" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
-        <v>1388</v>
+        <v>1681</v>
       </c>
       <c r="B312" t="s">
-        <v>1389</v>
+        <v>1682</v>
       </c>
       <c r="C312" t="s">
-        <v>1301</v>
+        <v>1592</v>
       </c>
       <c r="D312" t="s">
-        <v>1609</v>
+        <v>1683</v>
       </c>
       <c r="E312" t="s">
         <v>597</v>
       </c>
       <c r="F312">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G312">
-        <v>24.8</v>
+        <v>25.34</v>
       </c>
       <c r="H312" t="s">
-        <v>1391</v>
+        <v>1684</v>
       </c>
       <c r="I312" t="s">
-        <v>1392</v>
+        <v>1685</v>
       </c>
       <c r="J312" t="s">
-        <v>989</v>
+        <v>848</v>
       </c>
     </row>
     <row r="313" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
-        <v>1393</v>
+        <v>1686</v>
       </c>
       <c r="B313" t="s">
-        <v>1394</v>
+        <v>1687</v>
       </c>
       <c r="C313" t="s">
-        <v>1301</v>
+        <v>1592</v>
       </c>
       <c r="D313" t="s">
-        <v>1610</v>
+        <v>1688</v>
       </c>
       <c r="E313" t="s">
         <v>597</v>
       </c>
       <c r="F313">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G313">
-        <v>24.8</v>
+        <v>25.34</v>
       </c>
       <c r="H313" t="s">
-        <v>1396</v>
+        <v>1689</v>
       </c>
       <c r="I313" t="s">
-        <v>1397</v>
+        <v>1690</v>
       </c>
       <c r="J313" t="s">
-        <v>1000</v>
+        <v>854</v>
       </c>
     </row>
     <row r="314" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
-        <v>1398</v>
+        <v>1691</v>
       </c>
       <c r="B314" t="s">
-        <v>1399</v>
+        <v>1692</v>
       </c>
       <c r="C314" t="s">
-        <v>1301</v>
+        <v>1592</v>
       </c>
       <c r="D314" t="s">
-        <v>1611</v>
+        <v>1693</v>
       </c>
       <c r="E314" t="s">
         <v>597</v>
       </c>
       <c r="F314">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G314">
-        <v>24.8</v>
+        <v>25.34</v>
       </c>
       <c r="H314" t="s">
-        <v>1401</v>
+        <v>1694</v>
       </c>
       <c r="I314" t="s">
-        <v>1402</v>
+        <v>1695</v>
       </c>
       <c r="J314" t="s">
-        <v>740</v>
+        <v>860</v>
       </c>
     </row>
     <row r="315" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
-        <v>1403</v>
+        <v>1696</v>
       </c>
       <c r="B315" t="s">
-        <v>1404</v>
+        <v>1697</v>
       </c>
       <c r="C315" t="s">
-        <v>1301</v>
+        <v>1592</v>
       </c>
       <c r="D315" t="s">
-        <v>1612</v>
+        <v>1698</v>
       </c>
       <c r="E315" t="s">
         <v>597</v>
       </c>
       <c r="F315">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G315">
-        <v>24.8</v>
+        <v>25.34</v>
       </c>
       <c r="H315" t="s">
-        <v>1406</v>
+        <v>1699</v>
       </c>
       <c r="I315" t="s">
-        <v>1407</v>
+        <v>1700</v>
       </c>
       <c r="J315" t="s">
-        <v>746</v>
+        <v>866</v>
       </c>
     </row>
     <row r="316" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
-        <v>1408</v>
+        <v>1701</v>
       </c>
       <c r="B316" t="s">
-        <v>1409</v>
+        <v>1702</v>
       </c>
       <c r="C316" t="s">
-        <v>1301</v>
+        <v>1592</v>
       </c>
       <c r="D316" t="s">
-        <v>1613</v>
+        <v>1703</v>
       </c>
       <c r="E316" t="s">
         <v>597</v>
       </c>
       <c r="F316">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G316">
-        <v>24.8</v>
+        <v>25.34</v>
       </c>
       <c r="H316" t="s">
-        <v>1411</v>
+        <v>1704</v>
       </c>
       <c r="I316" t="s">
-        <v>1412</v>
+        <v>1705</v>
       </c>
       <c r="J316" t="s">
-        <v>1413</v>
+        <v>902</v>
       </c>
     </row>
     <row r="317" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
-        <v>1414</v>
+        <v>1706</v>
       </c>
       <c r="B317" t="s">
-        <v>1415</v>
+        <v>1707</v>
       </c>
       <c r="C317" t="s">
-        <v>1301</v>
+        <v>1592</v>
       </c>
       <c r="D317" t="s">
-        <v>1614</v>
+        <v>1708</v>
       </c>
       <c r="E317" t="s">
         <v>597</v>
       </c>
       <c r="F317">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G317">
-        <v>24.8</v>
+        <v>25.34</v>
       </c>
       <c r="H317" t="s">
-        <v>1417</v>
+        <v>1709</v>
       </c>
       <c r="I317" t="s">
-        <v>1418</v>
+        <v>1710</v>
       </c>
       <c r="J317" t="s">
-        <v>1051</v>
+        <v>1711</v>
       </c>
     </row>
     <row r="318" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
-        <v>1419</v>
+        <v>1712</v>
       </c>
       <c r="B318" t="s">
-        <v>1420</v>
+        <v>1713</v>
       </c>
       <c r="C318" t="s">
-        <v>1301</v>
+        <v>1592</v>
       </c>
       <c r="D318" t="s">
-        <v>1615</v>
+        <v>1714</v>
       </c>
       <c r="E318" t="s">
         <v>597</v>
       </c>
       <c r="F318">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G318">
-        <v>24.8</v>
+        <v>25.34</v>
       </c>
       <c r="H318" t="s">
-        <v>1422</v>
+        <v>1715</v>
       </c>
       <c r="I318" t="s">
-        <v>1423</v>
+        <v>1716</v>
       </c>
       <c r="J318" t="s">
-        <v>806</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="319" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
-        <v>1424</v>
+        <v>1717</v>
       </c>
       <c r="B319" t="s">
-        <v>1425</v>
+        <v>1718</v>
       </c>
       <c r="C319" t="s">
-        <v>1301</v>
+        <v>1592</v>
       </c>
       <c r="D319" t="s">
-        <v>1616</v>
+        <v>1719</v>
       </c>
       <c r="E319" t="s">
         <v>597</v>
       </c>
       <c r="F319">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G319">
-        <v>24.8</v>
+        <v>25.34</v>
       </c>
       <c r="H319" t="s">
-        <v>1427</v>
+        <v>1720</v>
       </c>
       <c r="I319" t="s">
-        <v>1428</v>
+        <v>1721</v>
       </c>
       <c r="J319" t="s">
-        <v>812</v>
-      </c>
-    </row>
-    <row r="320" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A320" t="s">
-        <v>1429</v>
-      </c>
-      <c r="B320" t="s">
-        <v>1430</v>
-      </c>
-      <c r="C320" t="s">
-        <v>1301</v>
-      </c>
-      <c r="D320" t="s">
-        <v>1617</v>
-      </c>
-      <c r="E320" t="s">
-        <v>597</v>
-      </c>
-      <c r="F320">
-        <v>48</v>
-      </c>
-      <c r="G320">
-        <v>24.8</v>
-      </c>
-      <c r="H320" t="s">
-        <v>1432</v>
-      </c>
-      <c r="I320" t="s">
-        <v>1433</v>
-      </c>
-      <c r="J320" t="s">
-        <v>818</v>
-      </c>
-    </row>
-    <row r="321" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A321" t="s">
-        <v>1434</v>
-      </c>
-      <c r="B321" t="s">
-        <v>1435</v>
-      </c>
-      <c r="C321" t="s">
-        <v>1301</v>
-      </c>
-      <c r="D321" t="s">
-        <v>1618</v>
-      </c>
-      <c r="E321" t="s">
-        <v>597</v>
-      </c>
-      <c r="F321">
-        <v>48</v>
-      </c>
-      <c r="G321">
-        <v>24.8</v>
-      </c>
-      <c r="H321" t="s">
-        <v>1437</v>
-      </c>
-      <c r="I321" t="s">
-        <v>1438</v>
-      </c>
-      <c r="J321" t="s">
-        <v>1094</v>
-      </c>
-    </row>
-    <row r="322" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A322" t="s">
-        <v>1439</v>
-      </c>
-      <c r="B322" t="s">
-        <v>1440</v>
-      </c>
-      <c r="C322" t="s">
-        <v>1301</v>
-      </c>
-      <c r="D322" t="s">
-        <v>1619</v>
-      </c>
-      <c r="E322" t="s">
-        <v>597</v>
-      </c>
-      <c r="F322">
-        <v>48</v>
-      </c>
-      <c r="G322">
-        <v>24.8</v>
-      </c>
-      <c r="H322" t="s">
-        <v>1442</v>
-      </c>
-      <c r="I322" t="s">
-        <v>1443</v>
-      </c>
-      <c r="J322" t="s">
-        <v>824</v>
-      </c>
-    </row>
-    <row r="323" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A323" t="s">
-        <v>1444</v>
-      </c>
-      <c r="B323" t="s">
-        <v>1445</v>
-      </c>
-      <c r="C323" t="s">
-        <v>1301</v>
-      </c>
-      <c r="D323" t="s">
-        <v>1620</v>
-      </c>
-      <c r="E323" t="s">
-        <v>597</v>
-      </c>
-      <c r="F323">
-        <v>48</v>
-      </c>
-      <c r="G323">
-        <v>24.8</v>
-      </c>
-      <c r="H323" t="s">
-        <v>1447</v>
-      </c>
-      <c r="I323" t="s">
-        <v>1448</v>
-      </c>
-      <c r="J323" t="s">
-        <v>830</v>
-      </c>
-    </row>
-    <row r="324" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A324" t="s">
-        <v>1449</v>
-      </c>
-      <c r="B324" t="s">
-        <v>1450</v>
-      </c>
-      <c r="C324" t="s">
-        <v>1301</v>
-      </c>
-      <c r="D324" t="s">
-        <v>1621</v>
-      </c>
-      <c r="E324" t="s">
-        <v>597</v>
-      </c>
-      <c r="F324">
-        <v>48</v>
-      </c>
-      <c r="G324">
-        <v>24.8</v>
-      </c>
-      <c r="H324" t="s">
-        <v>1452</v>
-      </c>
-      <c r="I324" t="s">
-        <v>1453</v>
-      </c>
-      <c r="J324" t="s">
-        <v>1454</v>
-      </c>
-    </row>
-    <row r="325" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A325" t="s">
-        <v>1455</v>
-      </c>
-      <c r="B325" t="s">
-        <v>1456</v>
-      </c>
-      <c r="C325" t="s">
-        <v>1301</v>
-      </c>
-      <c r="D325" t="s">
-        <v>1622</v>
-      </c>
-      <c r="E325" t="s">
-        <v>597</v>
-      </c>
-      <c r="F325">
-        <v>48</v>
-      </c>
-      <c r="G325">
-        <v>24.8</v>
-      </c>
-      <c r="H325" t="s">
-        <v>1458</v>
-      </c>
-      <c r="I325" t="s">
-        <v>1459</v>
-      </c>
-      <c r="J325" t="s">
-        <v>848</v>
-      </c>
-    </row>
-    <row r="326" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A326" t="s">
-        <v>1460</v>
-      </c>
-      <c r="B326" t="s">
-        <v>1461</v>
-      </c>
-      <c r="C326" t="s">
-        <v>1301</v>
-      </c>
-      <c r="D326" t="s">
-        <v>1623</v>
-      </c>
-      <c r="E326" t="s">
-        <v>597</v>
-      </c>
-      <c r="F326">
-        <v>48</v>
-      </c>
-      <c r="G326">
-        <v>24.8</v>
-      </c>
-      <c r="H326" t="s">
-        <v>1463</v>
-      </c>
-      <c r="I326" t="s">
-        <v>1464</v>
-      </c>
-      <c r="J326" t="s">
-        <v>854</v>
-      </c>
-    </row>
-    <row r="327" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A327" t="s">
-        <v>1465</v>
-      </c>
-      <c r="B327" t="s">
-        <v>1466</v>
-      </c>
-      <c r="C327" t="s">
-        <v>1301</v>
-      </c>
-      <c r="D327" t="s">
-        <v>1624</v>
-      </c>
-      <c r="E327" t="s">
-        <v>597</v>
-      </c>
-      <c r="F327">
-        <v>48</v>
-      </c>
-      <c r="G327">
-        <v>24.8</v>
-      </c>
-      <c r="H327" t="s">
-        <v>1468</v>
-      </c>
-      <c r="I327" t="s">
-        <v>1469</v>
-      </c>
-      <c r="J327" t="s">
-        <v>872</v>
-      </c>
-    </row>
-    <row r="328" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A328" t="s">
-        <v>1470</v>
-      </c>
-      <c r="B328" t="s">
-        <v>1471</v>
-      </c>
-      <c r="C328" t="s">
-        <v>1301</v>
-      </c>
-      <c r="D328" t="s">
-        <v>1625</v>
-      </c>
-      <c r="E328" t="s">
-        <v>597</v>
-      </c>
-      <c r="F328">
-        <v>48</v>
-      </c>
-      <c r="G328">
-        <v>24.8</v>
-      </c>
-      <c r="H328" t="s">
-        <v>1473</v>
-      </c>
-      <c r="I328" t="s">
-        <v>1474</v>
-      </c>
-      <c r="J328" t="s">
-        <v>1475</v>
-      </c>
-    </row>
-    <row r="329" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A329" t="s">
-        <v>1476</v>
-      </c>
-      <c r="B329" t="s">
-        <v>1477</v>
-      </c>
-      <c r="C329" t="s">
-        <v>1301</v>
-      </c>
-      <c r="D329" t="s">
-        <v>1626</v>
-      </c>
-      <c r="E329" t="s">
-        <v>597</v>
-      </c>
-      <c r="F329">
-        <v>48</v>
-      </c>
-      <c r="G329">
-        <v>24.8</v>
-      </c>
-      <c r="H329" t="s">
-        <v>1479</v>
-      </c>
-      <c r="I329" t="s">
-        <v>1480</v>
-      </c>
-      <c r="J329" t="s">
-        <v>1179</v>
-      </c>
-    </row>
-    <row r="330" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A330" t="s">
-        <v>1481</v>
-      </c>
-      <c r="B330" t="s">
-        <v>1482</v>
-      </c>
-      <c r="C330" t="s">
-        <v>1301</v>
-      </c>
-      <c r="D330" t="s">
-        <v>1627</v>
-      </c>
-      <c r="E330" t="s">
-        <v>597</v>
-      </c>
-      <c r="F330">
-        <v>48</v>
-      </c>
-      <c r="G330">
-        <v>24.8</v>
-      </c>
-      <c r="H330" t="s">
-        <v>1484</v>
-      </c>
-      <c r="I330" t="s">
-        <v>1485</v>
-      </c>
-      <c r="J330" t="s">
-        <v>1185</v>
-      </c>
-    </row>
-    <row r="331" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A331" t="s">
-        <v>1486</v>
-      </c>
-      <c r="B331" t="s">
-        <v>1487</v>
-      </c>
-      <c r="C331" t="s">
-        <v>1301</v>
-      </c>
-      <c r="D331" t="s">
-        <v>1628</v>
-      </c>
-      <c r="E331" t="s">
-        <v>597</v>
-      </c>
-      <c r="F331">
-        <v>48</v>
-      </c>
-      <c r="G331">
-        <v>24.8</v>
-      </c>
-      <c r="H331" t="s">
-        <v>1489</v>
-      </c>
-      <c r="I331" t="s">
-        <v>1490</v>
-      </c>
-      <c r="J331" t="s">
-        <v>1191</v>
-      </c>
-    </row>
-    <row r="332" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A332" t="s">
-        <v>1491</v>
-      </c>
-      <c r="B332" t="s">
-        <v>1492</v>
-      </c>
-      <c r="C332" t="s">
-        <v>1301</v>
-      </c>
-      <c r="D332" t="s">
-        <v>1629</v>
-      </c>
-      <c r="E332" t="s">
-        <v>597</v>
-      </c>
-      <c r="F332">
-        <v>48</v>
-      </c>
-      <c r="G332">
-        <v>24.8</v>
-      </c>
-      <c r="H332" t="s">
-        <v>1494</v>
-      </c>
-      <c r="I332" t="s">
-        <v>1495</v>
-      </c>
-      <c r="J332" t="s">
-        <v>1197</v>
-      </c>
-    </row>
-    <row r="333" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A333" t="s">
-        <v>1496</v>
-      </c>
-      <c r="B333" t="s">
-        <v>1497</v>
-      </c>
-      <c r="C333" t="s">
-        <v>1301</v>
-      </c>
-      <c r="D333" t="s">
-        <v>1630</v>
-      </c>
-      <c r="E333" t="s">
-        <v>597</v>
-      </c>
-      <c r="F333">
-        <v>48</v>
-      </c>
-      <c r="G333">
-        <v>24.8</v>
-      </c>
-      <c r="H333" t="s">
-        <v>1499</v>
-      </c>
-      <c r="I333" t="s">
-        <v>1500</v>
-      </c>
-      <c r="J333" t="s">
-        <v>1203</v>
-      </c>
-    </row>
-    <row r="334" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A334" t="s">
-        <v>1501</v>
-      </c>
-      <c r="B334" t="s">
-        <v>1502</v>
-      </c>
-      <c r="C334" t="s">
-        <v>1301</v>
-      </c>
-      <c r="D334" t="s">
-        <v>1631</v>
-      </c>
-      <c r="E334" t="s">
-        <v>597</v>
-      </c>
-      <c r="F334">
-        <v>48</v>
-      </c>
-      <c r="G334">
-        <v>24.8</v>
-      </c>
-      <c r="H334" t="s">
-        <v>1504</v>
-      </c>
-      <c r="I334" t="s">
-        <v>1505</v>
-      </c>
-      <c r="J334" t="s">
-        <v>1506</v>
-      </c>
-    </row>
-    <row r="335" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A335" t="s">
-        <v>1507</v>
-      </c>
-      <c r="B335" t="s">
-        <v>1508</v>
-      </c>
-      <c r="C335" t="s">
-        <v>1301</v>
-      </c>
-      <c r="D335" t="s">
-        <v>1632</v>
-      </c>
-      <c r="E335" t="s">
-        <v>597</v>
-      </c>
-      <c r="F335">
-        <v>48</v>
-      </c>
-      <c r="G335">
-        <v>24.8</v>
-      </c>
-      <c r="H335" t="s">
-        <v>1510</v>
-      </c>
-      <c r="I335" t="s">
-        <v>1511</v>
-      </c>
-      <c r="J335" t="s">
-        <v>1512</v>
-      </c>
-    </row>
-    <row r="336" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A336" t="s">
-        <v>1513</v>
-      </c>
-      <c r="B336" t="s">
-        <v>1514</v>
-      </c>
-      <c r="C336" t="s">
-        <v>1301</v>
-      </c>
-      <c r="D336" t="s">
-        <v>1633</v>
-      </c>
-      <c r="E336" t="s">
-        <v>597</v>
-      </c>
-      <c r="F336">
-        <v>48</v>
-      </c>
-      <c r="G336">
-        <v>24.8</v>
-      </c>
-      <c r="H336" t="s">
-        <v>1516</v>
-      </c>
-      <c r="I336" t="s">
-        <v>1517</v>
-      </c>
-      <c r="J336" t="s">
-        <v>1518</v>
-      </c>
-    </row>
-    <row r="337" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A337" t="s">
-        <v>1519</v>
-      </c>
-      <c r="B337" t="s">
-        <v>1520</v>
-      </c>
-      <c r="C337" t="s">
-        <v>1301</v>
-      </c>
-      <c r="D337" t="s">
-        <v>1634</v>
-      </c>
-      <c r="E337" t="s">
-        <v>597</v>
-      </c>
-      <c r="F337">
-        <v>48</v>
-      </c>
-      <c r="G337">
-        <v>24.8</v>
-      </c>
-      <c r="H337" t="s">
-        <v>1522</v>
-      </c>
-      <c r="I337" t="s">
-        <v>1523</v>
-      </c>
-      <c r="J337" t="s">
-        <v>1226</v>
-      </c>
-    </row>
-    <row r="338" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A338" t="s">
-        <v>1524</v>
-      </c>
-      <c r="B338" t="s">
-        <v>1525</v>
-      </c>
-      <c r="C338" t="s">
-        <v>1301</v>
-      </c>
-      <c r="D338" t="s">
-        <v>1635</v>
-      </c>
-      <c r="E338" t="s">
-        <v>597</v>
-      </c>
-      <c r="F338">
-        <v>48</v>
-      </c>
-      <c r="G338">
-        <v>24.8</v>
-      </c>
-      <c r="H338" t="s">
-        <v>1527</v>
-      </c>
-      <c r="I338" t="s">
-        <v>1528</v>
-      </c>
-      <c r="J338" t="s">
-        <v>1232</v>
-      </c>
-    </row>
-    <row r="339" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A339" t="s">
-        <v>1529</v>
-      </c>
-      <c r="B339" t="s">
-        <v>1530</v>
-      </c>
-      <c r="C339" t="s">
-        <v>1301</v>
-      </c>
-      <c r="D339" t="s">
-        <v>1636</v>
-      </c>
-      <c r="E339" t="s">
-        <v>597</v>
-      </c>
-      <c r="F339">
-        <v>48</v>
-      </c>
-      <c r="G339">
-        <v>24.8</v>
-      </c>
-      <c r="H339" t="s">
-        <v>1532</v>
-      </c>
-      <c r="I339" t="s">
-        <v>1533</v>
-      </c>
-      <c r="J339" t="s">
-        <v>1238</v>
-      </c>
-    </row>
-    <row r="340" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A340" t="s">
-        <v>1534</v>
-      </c>
-      <c r="B340" t="s">
-        <v>1535</v>
-      </c>
-      <c r="C340" t="s">
-        <v>1301</v>
-      </c>
-      <c r="D340" t="s">
-        <v>1637</v>
-      </c>
-      <c r="E340" t="s">
-        <v>597</v>
-      </c>
-      <c r="F340">
-        <v>48</v>
-      </c>
-      <c r="G340">
-        <v>24.8</v>
-      </c>
-      <c r="H340" t="s">
-        <v>1537</v>
-      </c>
-      <c r="I340" t="s">
-        <v>1538</v>
-      </c>
-      <c r="J340" t="s">
-        <v>1244</v>
-      </c>
-    </row>
-    <row r="341" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A341" t="s">
-        <v>1539</v>
-      </c>
-      <c r="B341" t="s">
-        <v>1540</v>
-      </c>
-      <c r="C341" t="s">
-        <v>1301</v>
-      </c>
-      <c r="D341" t="s">
-        <v>1638</v>
-      </c>
-      <c r="E341" t="s">
-        <v>597</v>
-      </c>
-      <c r="F341">
-        <v>48</v>
-      </c>
-      <c r="G341">
-        <v>24.8</v>
-      </c>
-      <c r="H341" t="s">
-        <v>1542</v>
-      </c>
-      <c r="I341" t="s">
-        <v>1543</v>
-      </c>
-      <c r="J341" t="s">
-        <v>1544</v>
-      </c>
-    </row>
-    <row r="342" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A342" t="s">
-        <v>1545</v>
-      </c>
-      <c r="B342" t="s">
-        <v>1546</v>
-      </c>
-      <c r="C342" t="s">
-        <v>1301</v>
-      </c>
-      <c r="D342" t="s">
-        <v>1639</v>
-      </c>
-      <c r="E342" t="s">
-        <v>597</v>
-      </c>
-      <c r="F342">
-        <v>48</v>
-      </c>
-      <c r="G342">
-        <v>24.8</v>
-      </c>
-      <c r="H342" t="s">
-        <v>1548</v>
-      </c>
-      <c r="I342" t="s">
-        <v>1549</v>
-      </c>
-      <c r="J342" t="s">
-        <v>1250</v>
-      </c>
-    </row>
-    <row r="343" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A343" t="s">
-        <v>1550</v>
-      </c>
-      <c r="B343" t="s">
-        <v>1551</v>
-      </c>
-      <c r="C343" t="s">
-        <v>1301</v>
-      </c>
-      <c r="D343" t="s">
-        <v>1640</v>
-      </c>
-      <c r="E343" t="s">
-        <v>597</v>
-      </c>
-      <c r="F343">
-        <v>48</v>
-      </c>
-      <c r="G343">
-        <v>24.8</v>
-      </c>
-      <c r="H343" t="s">
-        <v>1553</v>
-      </c>
-      <c r="I343" t="s">
-        <v>1554</v>
-      </c>
-      <c r="J343" t="s">
-        <v>1256</v>
-      </c>
-    </row>
-    <row r="344" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A344" t="s">
-        <v>1555</v>
-      </c>
-      <c r="B344" t="s">
-        <v>1556</v>
-      </c>
-      <c r="C344" t="s">
-        <v>1301</v>
-      </c>
-      <c r="D344" t="s">
-        <v>1641</v>
-      </c>
-      <c r="E344" t="s">
-        <v>597</v>
-      </c>
-      <c r="F344">
-        <v>48</v>
-      </c>
-      <c r="G344">
-        <v>24.8</v>
-      </c>
-      <c r="H344" t="s">
-        <v>1558</v>
-      </c>
-      <c r="I344" t="s">
-        <v>1559</v>
-      </c>
-      <c r="J344" t="s">
-        <v>1262</v>
-      </c>
-    </row>
-    <row r="345" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A345" t="s">
-        <v>1560</v>
-      </c>
-      <c r="B345" t="s">
-        <v>1561</v>
-      </c>
-      <c r="C345" t="s">
-        <v>1301</v>
-      </c>
-      <c r="D345" t="s">
-        <v>1642</v>
-      </c>
-      <c r="E345" t="s">
-        <v>597</v>
-      </c>
-      <c r="F345">
-        <v>48</v>
-      </c>
-      <c r="G345">
-        <v>24.8</v>
-      </c>
-      <c r="H345" t="s">
-        <v>1563</v>
-      </c>
-      <c r="I345" t="s">
-        <v>1564</v>
-      </c>
-      <c r="J345" t="s">
-        <v>1268</v>
-      </c>
-    </row>
-    <row r="346" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A346" t="s">
-        <v>1565</v>
-      </c>
-      <c r="B346" t="s">
-        <v>1566</v>
-      </c>
-      <c r="C346" t="s">
-        <v>1301</v>
-      </c>
-      <c r="D346" t="s">
-        <v>1643</v>
-      </c>
-      <c r="E346" t="s">
-        <v>597</v>
-      </c>
-      <c r="F346">
-        <v>48</v>
-      </c>
-      <c r="G346">
-        <v>24.8</v>
-      </c>
-      <c r="H346" t="s">
-        <v>1568</v>
-      </c>
-      <c r="I346" t="s">
-        <v>1569</v>
-      </c>
-      <c r="J346" t="s">
-        <v>1274</v>
-      </c>
-    </row>
-    <row r="347" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A347" t="s">
-        <v>1570</v>
-      </c>
-      <c r="B347" t="s">
-        <v>1571</v>
-      </c>
-      <c r="C347" t="s">
-        <v>1301</v>
-      </c>
-      <c r="D347" t="s">
-        <v>1644</v>
-      </c>
-      <c r="E347" t="s">
-        <v>597</v>
-      </c>
-      <c r="F347">
-        <v>48</v>
-      </c>
-      <c r="G347">
-        <v>24.8</v>
-      </c>
-      <c r="H347" t="s">
-        <v>1573</v>
-      </c>
-      <c r="I347" t="s">
-        <v>1574</v>
-      </c>
-      <c r="J347" t="s">
-        <v>1280</v>
-      </c>
-    </row>
-    <row r="348" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A348" t="s">
-        <v>1575</v>
-      </c>
-      <c r="B348" t="s">
-        <v>1576</v>
-      </c>
-      <c r="C348" t="s">
-        <v>1301</v>
-      </c>
-      <c r="D348" t="s">
-        <v>1645</v>
-      </c>
-      <c r="E348" t="s">
-        <v>597</v>
-      </c>
-      <c r="F348">
-        <v>48</v>
-      </c>
-      <c r="G348">
-        <v>24.8</v>
-      </c>
-      <c r="H348" t="s">
-        <v>1578</v>
-      </c>
-      <c r="I348" t="s">
-        <v>1579</v>
-      </c>
-      <c r="J348" t="s">
-        <v>1286</v>
-      </c>
-    </row>
-    <row r="349" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A349" t="s">
-        <v>1580</v>
-      </c>
-      <c r="B349" t="s">
-        <v>1581</v>
-      </c>
-      <c r="C349" t="s">
-        <v>1301</v>
-      </c>
-      <c r="D349" t="s">
-        <v>1646</v>
-      </c>
-      <c r="E349" t="s">
-        <v>597</v>
-      </c>
-      <c r="F349">
-        <v>48</v>
-      </c>
-      <c r="G349">
-        <v>24.8</v>
-      </c>
-      <c r="H349" t="s">
-        <v>1583</v>
-      </c>
-      <c r="I349" t="s">
-        <v>1584</v>
-      </c>
-      <c r="J349" t="s">
-        <v>1585</v>
-      </c>
-    </row>
-    <row r="350" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A350" t="s">
-        <v>1586</v>
-      </c>
-      <c r="B350" t="s">
-        <v>1587</v>
-      </c>
-      <c r="C350" t="s">
-        <v>1301</v>
-      </c>
-      <c r="D350" t="s">
-        <v>1647</v>
-      </c>
-      <c r="E350" t="s">
-        <v>597</v>
-      </c>
-      <c r="F350">
-        <v>48</v>
-      </c>
-      <c r="G350">
-        <v>24.8</v>
-      </c>
-      <c r="H350" t="s">
-        <v>1589</v>
-      </c>
-      <c r="I350" t="s">
-        <v>1590</v>
-      </c>
-      <c r="J350" t="s">
-        <v>1591</v>
-      </c>
-    </row>
-    <row r="351" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A351" t="s">
-        <v>1648</v>
-      </c>
-      <c r="B351" t="s">
-        <v>1649</v>
-      </c>
-      <c r="C351" t="s">
-        <v>1650</v>
-      </c>
-      <c r="D351" t="s">
-        <v>1650</v>
-      </c>
-      <c r="E351" t="s">
-        <v>597</v>
-      </c>
-      <c r="F351">
-        <v>41</v>
-      </c>
-      <c r="G351">
-        <v>25.34</v>
-      </c>
-      <c r="H351" t="s">
-        <v>1651</v>
-      </c>
-      <c r="I351" t="s">
-        <v>1652</v>
-      </c>
-      <c r="J351" t="s">
-        <v>1653</v>
-      </c>
-    </row>
-    <row r="352" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A352" t="s">
-        <v>1654</v>
-      </c>
-      <c r="B352" t="s">
-        <v>1655</v>
-      </c>
-      <c r="C352" t="s">
-        <v>1650</v>
-      </c>
-      <c r="D352" t="s">
-        <v>1656</v>
-      </c>
-      <c r="E352" t="s">
-        <v>597</v>
-      </c>
-      <c r="F352">
-        <v>41</v>
-      </c>
-      <c r="G352">
-        <v>25.34</v>
-      </c>
-      <c r="H352" t="s">
-        <v>1657</v>
-      </c>
-      <c r="I352" t="s">
-        <v>1658</v>
-      </c>
-      <c r="J352" t="s">
-        <v>1659</v>
-      </c>
-    </row>
-    <row r="353" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A353" t="s">
-        <v>1660</v>
-      </c>
-      <c r="B353" t="s">
-        <v>1661</v>
-      </c>
-      <c r="C353" t="s">
-        <v>1650</v>
-      </c>
-      <c r="D353" t="s">
-        <v>1662</v>
-      </c>
-      <c r="E353" t="s">
-        <v>597</v>
-      </c>
-      <c r="F353">
-        <v>41</v>
-      </c>
-      <c r="G353">
-        <v>25.34</v>
-      </c>
-      <c r="H353" t="s">
-        <v>1663</v>
-      </c>
-      <c r="I353" t="s">
-        <v>1664</v>
-      </c>
-      <c r="J353" t="s">
-        <v>1665</v>
-      </c>
-    </row>
-    <row r="354" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A354" t="s">
-        <v>1666</v>
-      </c>
-      <c r="B354" t="s">
-        <v>1667</v>
-      </c>
-      <c r="C354" t="s">
-        <v>1650</v>
-      </c>
-      <c r="D354" t="s">
-        <v>1668</v>
-      </c>
-      <c r="E354" t="s">
-        <v>597</v>
-      </c>
-      <c r="F354">
-        <v>41</v>
-      </c>
-      <c r="G354">
-        <v>25.34</v>
-      </c>
-      <c r="H354" t="s">
-        <v>1669</v>
-      </c>
-      <c r="I354" t="s">
-        <v>1670</v>
-      </c>
-      <c r="J354" t="s">
-        <v>1671</v>
-      </c>
-    </row>
-    <row r="355" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A355" t="s">
-        <v>1672</v>
-      </c>
-      <c r="B355" t="s">
-        <v>1673</v>
-      </c>
-      <c r="C355" t="s">
-        <v>1650</v>
-      </c>
-      <c r="D355" t="s">
-        <v>1674</v>
-      </c>
-      <c r="E355" t="s">
-        <v>597</v>
-      </c>
-      <c r="F355">
-        <v>41</v>
-      </c>
-      <c r="G355">
-        <v>25.34</v>
-      </c>
-      <c r="H355" t="s">
-        <v>1675</v>
-      </c>
-      <c r="I355" t="s">
-        <v>1676</v>
-      </c>
-      <c r="J355" t="s">
-        <v>1677</v>
-      </c>
-    </row>
-    <row r="356" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A356" t="s">
-        <v>1678</v>
-      </c>
-      <c r="B356" t="s">
-        <v>1679</v>
-      </c>
-      <c r="C356" t="s">
-        <v>1650</v>
-      </c>
-      <c r="D356" t="s">
-        <v>1680</v>
-      </c>
-      <c r="E356" t="s">
-        <v>597</v>
-      </c>
-      <c r="F356">
-        <v>41</v>
-      </c>
-      <c r="G356">
-        <v>25.34</v>
-      </c>
-      <c r="H356" t="s">
-        <v>1681</v>
-      </c>
-      <c r="I356" t="s">
-        <v>1682</v>
-      </c>
-      <c r="J356" t="s">
-        <v>1683</v>
-      </c>
-    </row>
-    <row r="357" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A357" t="s">
-        <v>1684</v>
-      </c>
-      <c r="B357" t="s">
-        <v>1685</v>
-      </c>
-      <c r="C357" t="s">
-        <v>1650</v>
-      </c>
-      <c r="D357" t="s">
-        <v>1686</v>
-      </c>
-      <c r="E357" t="s">
-        <v>597</v>
-      </c>
-      <c r="F357">
-        <v>41</v>
-      </c>
-      <c r="G357">
-        <v>25.34</v>
-      </c>
-      <c r="H357" t="s">
-        <v>1687</v>
-      </c>
-      <c r="I357" t="s">
-        <v>1688</v>
-      </c>
-      <c r="J357" t="s">
-        <v>954</v>
-      </c>
-    </row>
-    <row r="358" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A358" t="s">
-        <v>1689</v>
-      </c>
-      <c r="B358" t="s">
-        <v>1690</v>
-      </c>
-      <c r="C358" t="s">
-        <v>1650</v>
-      </c>
-      <c r="D358" t="s">
-        <v>1691</v>
-      </c>
-      <c r="E358" t="s">
-        <v>597</v>
-      </c>
-      <c r="F358">
-        <v>41</v>
-      </c>
-      <c r="G358">
-        <v>25.34</v>
-      </c>
-      <c r="H358" t="s">
-        <v>1692</v>
-      </c>
-      <c r="I358" t="s">
-        <v>1693</v>
-      </c>
-      <c r="J358" t="s">
-        <v>680</v>
-      </c>
-    </row>
-    <row r="359" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A359" t="s">
-        <v>1694</v>
-      </c>
-      <c r="B359" t="s">
-        <v>1695</v>
-      </c>
-      <c r="C359" t="s">
-        <v>1650</v>
-      </c>
-      <c r="D359" t="s">
-        <v>1696</v>
-      </c>
-      <c r="E359" t="s">
-        <v>597</v>
-      </c>
-      <c r="F359">
-        <v>41</v>
-      </c>
-      <c r="G359">
-        <v>25.34</v>
-      </c>
-      <c r="H359" t="s">
-        <v>1697</v>
-      </c>
-      <c r="I359" t="s">
-        <v>1698</v>
-      </c>
-      <c r="J359" t="s">
-        <v>686</v>
-      </c>
-    </row>
-    <row r="360" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A360" t="s">
-        <v>1699</v>
-      </c>
-      <c r="B360" t="s">
-        <v>1700</v>
-      </c>
-      <c r="C360" t="s">
-        <v>1650</v>
-      </c>
-      <c r="D360" t="s">
-        <v>1701</v>
-      </c>
-      <c r="E360" t="s">
-        <v>597</v>
-      </c>
-      <c r="F360">
-        <v>41</v>
-      </c>
-      <c r="G360">
-        <v>25.34</v>
-      </c>
-      <c r="H360" t="s">
-        <v>1702</v>
-      </c>
-      <c r="I360" t="s">
-        <v>1703</v>
-      </c>
-      <c r="J360" t="s">
-        <v>692</v>
-      </c>
-    </row>
-    <row r="361" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A361" t="s">
-        <v>1704</v>
-      </c>
-      <c r="B361" t="s">
-        <v>1705</v>
-      </c>
-      <c r="C361" t="s">
-        <v>1650</v>
-      </c>
-      <c r="D361" t="s">
-        <v>1706</v>
-      </c>
-      <c r="E361" t="s">
-        <v>597</v>
-      </c>
-      <c r="F361">
-        <v>41</v>
-      </c>
-      <c r="G361">
-        <v>25.34</v>
-      </c>
-      <c r="H361" t="s">
-        <v>1707</v>
-      </c>
-      <c r="I361" t="s">
-        <v>1708</v>
-      </c>
-      <c r="J361" t="s">
-        <v>698</v>
-      </c>
-    </row>
-    <row r="362" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A362" t="s">
-        <v>1709</v>
-      </c>
-      <c r="B362" t="s">
-        <v>1710</v>
-      </c>
-      <c r="C362" t="s">
-        <v>1650</v>
-      </c>
-      <c r="D362" t="s">
-        <v>1711</v>
-      </c>
-      <c r="E362" t="s">
-        <v>597</v>
-      </c>
-      <c r="F362">
-        <v>41</v>
-      </c>
-      <c r="G362">
-        <v>25.34</v>
-      </c>
-      <c r="H362" t="s">
-        <v>1712</v>
-      </c>
-      <c r="I362" t="s">
-        <v>1713</v>
-      </c>
-      <c r="J362" t="s">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="363" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A363" t="s">
-        <v>1714</v>
-      </c>
-      <c r="B363" t="s">
-        <v>1715</v>
-      </c>
-      <c r="C363" t="s">
-        <v>1650</v>
-      </c>
-      <c r="D363" t="s">
-        <v>1716</v>
-      </c>
-      <c r="E363" t="s">
-        <v>597</v>
-      </c>
-      <c r="F363">
-        <v>41</v>
-      </c>
-      <c r="G363">
-        <v>25.34</v>
-      </c>
-      <c r="H363" t="s">
-        <v>1717</v>
-      </c>
-      <c r="I363" t="s">
-        <v>1718</v>
-      </c>
-      <c r="J363" t="s">
-        <v>746</v>
-      </c>
-    </row>
-    <row r="364" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A364" t="s">
-        <v>1719</v>
-      </c>
-      <c r="B364" t="s">
-        <v>1720</v>
-      </c>
-      <c r="C364" t="s">
-        <v>1650</v>
-      </c>
-      <c r="D364" t="s">
-        <v>1721</v>
-      </c>
-      <c r="E364" t="s">
-        <v>597</v>
-      </c>
-      <c r="F364">
-        <v>41</v>
-      </c>
-      <c r="G364">
-        <v>25.34</v>
-      </c>
-      <c r="H364" t="s">
-        <v>1722</v>
-      </c>
-      <c r="I364" t="s">
-        <v>1723</v>
-      </c>
-      <c r="J364" t="s">
-        <v>806</v>
-      </c>
-    </row>
-    <row r="365" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A365" t="s">
-        <v>1724</v>
-      </c>
-      <c r="B365" t="s">
-        <v>1725</v>
-      </c>
-      <c r="C365" t="s">
-        <v>1650</v>
-      </c>
-      <c r="D365" t="s">
-        <v>1726</v>
-      </c>
-      <c r="E365" t="s">
-        <v>597</v>
-      </c>
-      <c r="F365">
-        <v>41</v>
-      </c>
-      <c r="G365">
-        <v>25.34</v>
-      </c>
-      <c r="H365" t="s">
-        <v>1727</v>
-      </c>
-      <c r="I365" t="s">
-        <v>1728</v>
-      </c>
-      <c r="J365" t="s">
-        <v>812</v>
-      </c>
-    </row>
-    <row r="366" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A366" t="s">
-        <v>1729</v>
-      </c>
-      <c r="B366" t="s">
-        <v>1730</v>
-      </c>
-      <c r="C366" t="s">
-        <v>1650</v>
-      </c>
-      <c r="D366" t="s">
-        <v>1731</v>
-      </c>
-      <c r="E366" t="s">
-        <v>597</v>
-      </c>
-      <c r="F366">
-        <v>41</v>
-      </c>
-      <c r="G366">
-        <v>25.34</v>
-      </c>
-      <c r="H366" t="s">
-        <v>1732</v>
-      </c>
-      <c r="I366" t="s">
-        <v>1733</v>
-      </c>
-      <c r="J366" t="s">
-        <v>1082</v>
-      </c>
-    </row>
-    <row r="367" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A367" t="s">
-        <v>1734</v>
-      </c>
-      <c r="B367" t="s">
-        <v>1735</v>
-      </c>
-      <c r="C367" t="s">
-        <v>1650</v>
-      </c>
-      <c r="D367" t="s">
-        <v>1736</v>
-      </c>
-      <c r="E367" t="s">
-        <v>597</v>
-      </c>
-      <c r="F367">
-        <v>41</v>
-      </c>
-      <c r="G367">
-        <v>25.34</v>
-      </c>
-      <c r="H367" t="s">
-        <v>1737</v>
-      </c>
-      <c r="I367" t="s">
-        <v>1738</v>
-      </c>
-      <c r="J367" t="s">
-        <v>1088</v>
-      </c>
-    </row>
-    <row r="368" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A368" t="s">
-        <v>1739</v>
-      </c>
-      <c r="B368" t="s">
-        <v>1740</v>
-      </c>
-      <c r="C368" t="s">
-        <v>1650</v>
-      </c>
-      <c r="D368" t="s">
-        <v>1741</v>
-      </c>
-      <c r="E368" t="s">
-        <v>597</v>
-      </c>
-      <c r="F368">
-        <v>41</v>
-      </c>
-      <c r="G368">
-        <v>25.34</v>
-      </c>
-      <c r="H368" t="s">
-        <v>1742</v>
-      </c>
-      <c r="I368" t="s">
-        <v>1743</v>
-      </c>
-      <c r="J368" t="s">
-        <v>848</v>
-      </c>
-    </row>
-    <row r="369" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A369" t="s">
-        <v>1744</v>
-      </c>
-      <c r="B369" t="s">
-        <v>1745</v>
-      </c>
-      <c r="C369" t="s">
-        <v>1650</v>
-      </c>
-      <c r="D369" t="s">
-        <v>1746</v>
-      </c>
-      <c r="E369" t="s">
-        <v>597</v>
-      </c>
-      <c r="F369">
-        <v>41</v>
-      </c>
-      <c r="G369">
-        <v>25.34</v>
-      </c>
-      <c r="H369" t="s">
-        <v>1747</v>
-      </c>
-      <c r="I369" t="s">
-        <v>1748</v>
-      </c>
-      <c r="J369" t="s">
-        <v>854</v>
-      </c>
-    </row>
-    <row r="370" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A370" t="s">
-        <v>1749</v>
-      </c>
-      <c r="B370" t="s">
-        <v>1750</v>
-      </c>
-      <c r="C370" t="s">
-        <v>1650</v>
-      </c>
-      <c r="D370" t="s">
-        <v>1751</v>
-      </c>
-      <c r="E370" t="s">
-        <v>597</v>
-      </c>
-      <c r="F370">
-        <v>41</v>
-      </c>
-      <c r="G370">
-        <v>25.34</v>
-      </c>
-      <c r="H370" t="s">
-        <v>1752</v>
-      </c>
-      <c r="I370" t="s">
-        <v>1753</v>
-      </c>
-      <c r="J370" t="s">
-        <v>860</v>
-      </c>
-    </row>
-    <row r="371" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A371" t="s">
-        <v>1754</v>
-      </c>
-      <c r="B371" t="s">
-        <v>1755</v>
-      </c>
-      <c r="C371" t="s">
-        <v>1650</v>
-      </c>
-      <c r="D371" t="s">
-        <v>1756</v>
-      </c>
-      <c r="E371" t="s">
-        <v>597</v>
-      </c>
-      <c r="F371">
-        <v>41</v>
-      </c>
-      <c r="G371">
-        <v>25.34</v>
-      </c>
-      <c r="H371" t="s">
-        <v>1757</v>
-      </c>
-      <c r="I371" t="s">
-        <v>1758</v>
-      </c>
-      <c r="J371" t="s">
-        <v>866</v>
-      </c>
-    </row>
-    <row r="372" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A372" t="s">
-        <v>1759</v>
-      </c>
-      <c r="B372" t="s">
-        <v>1760</v>
-      </c>
-      <c r="C372" t="s">
-        <v>1650</v>
-      </c>
-      <c r="D372" t="s">
-        <v>1761</v>
-      </c>
-      <c r="E372" t="s">
-        <v>597</v>
-      </c>
-      <c r="F372">
-        <v>41</v>
-      </c>
-      <c r="G372">
-        <v>25.34</v>
-      </c>
-      <c r="H372" t="s">
-        <v>1762</v>
-      </c>
-      <c r="I372" t="s">
-        <v>1763</v>
-      </c>
-      <c r="J372" t="s">
-        <v>902</v>
-      </c>
-    </row>
-    <row r="373" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A373" t="s">
-        <v>1764</v>
-      </c>
-      <c r="B373" t="s">
-        <v>1765</v>
-      </c>
-      <c r="C373" t="s">
-        <v>1650</v>
-      </c>
-      <c r="D373" t="s">
-        <v>1766</v>
-      </c>
-      <c r="E373" t="s">
-        <v>597</v>
-      </c>
-      <c r="F373">
-        <v>41</v>
-      </c>
-      <c r="G373">
-        <v>25.34</v>
-      </c>
-      <c r="H373" t="s">
-        <v>1767</v>
-      </c>
-      <c r="I373" t="s">
-        <v>1768</v>
-      </c>
-      <c r="J373" t="s">
-        <v>1769</v>
-      </c>
-    </row>
-    <row r="374" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A374" t="s">
-        <v>1770</v>
-      </c>
-      <c r="B374" t="s">
-        <v>1771</v>
-      </c>
-      <c r="C374" t="s">
-        <v>1650</v>
-      </c>
-      <c r="D374" t="s">
-        <v>1772</v>
-      </c>
-      <c r="E374" t="s">
-        <v>597</v>
-      </c>
-      <c r="F374">
-        <v>41</v>
-      </c>
-      <c r="G374">
-        <v>25.34</v>
-      </c>
-      <c r="H374" t="s">
-        <v>1773</v>
-      </c>
-      <c r="I374" t="s">
-        <v>1774</v>
-      </c>
-      <c r="J374" t="s">
-        <v>1268</v>
-      </c>
-    </row>
-    <row r="375" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A375" t="s">
-        <v>1775</v>
-      </c>
-      <c r="B375" t="s">
-        <v>1776</v>
-      </c>
-      <c r="C375" t="s">
-        <v>1650</v>
-      </c>
-      <c r="D375" t="s">
-        <v>1777</v>
-      </c>
-      <c r="E375" t="s">
-        <v>597</v>
-      </c>
-      <c r="F375">
-        <v>41</v>
-      </c>
-      <c r="G375">
-        <v>25.34</v>
-      </c>
-      <c r="H375" t="s">
-        <v>1778</v>
-      </c>
-      <c r="I375" t="s">
-        <v>1779</v>
-      </c>
-      <c r="J375" t="s">
         <v>1274</v>
       </c>
     </row>
@@ -17817,6 +15858,9 @@
     <hyperlink ref="J215" r:id="rId12" location="16" xr:uid="{F1E6EF78-6CE8-D146-9960-6A4FCE23FDEC}"/>
     <hyperlink ref="J216" r:id="rId13" location="16" xr:uid="{09452BD4-EB49-E74C-9DC2-8F0CC5B79C1A}"/>
     <hyperlink ref="J225" r:id="rId14" location="19" xr:uid="{DB6A0B2A-3C5C-F74F-B694-8502B717A4DD}"/>
+    <hyperlink ref="H245" r:id="rId15" xr:uid="{76ABDAE1-C08A-844E-8A4B-69E609C74D95}"/>
+    <hyperlink ref="J245" r:id="rId16" location="3A" xr:uid="{6488783D-809A-E542-8761-E7BAF8D50FBB}"/>
+    <hyperlink ref="J246" r:id="rId17" location="3A" xr:uid="{862591C8-2B48-DF44-9E00-D937D9AD43B0}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>